<commit_message>
2019.10.08. 김동욱 PSP 수정
</commit_message>
<xml_diff>
--- a/4팀_PSP_Sheet.xlsx
+++ b/4팀_PSP_Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyriloe/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsung\Desktop\강의 등\github\filling good\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362FA5AC-C9D6-3A4E-B355-08D3CB401F38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020FF31B-4ED3-4AB6-9A28-356FBB3E0455}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="1740" windowWidth="23240" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="총합" sheetId="1" r:id="rId1"/>
@@ -1480,7 +1480,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="51">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -1812,6 +1812,26 @@
   </si>
   <si>
     <t>Prototyping을 위한 안드로이드 SharedPreference 기능 스터디</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>usecase diagram 작성</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>usecase 및 prototype 작성 관련 조모임</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>spec 작성 관련 조모임</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>추천 시스템 탐색 및 스터디</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>usecase outline 수정 및 specification 작성</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2421,17 +2441,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="7" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="46.5" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="46.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="11.75" customHeight="1">
@@ -2462,7 +2482,7 @@
       <c r="E3"/>
     </row>
     <row r="4" spans="1:6" ht="11.75" customHeight="1"/>
-    <row r="5" spans="1:6" s="10" customFormat="1" ht="28">
+    <row r="5" spans="1:6" s="10" customFormat="1" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -2763,7 +2783,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2780,7 +2800,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2797,7 +2817,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2814,7 +2834,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2831,7 +2851,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2848,7 +2868,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2865,7 +2885,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2881,17 +2901,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="49.5" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" customWidth="1"/>
+    <col min="6" max="6" width="49.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -2908,7 +2928,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="16">
+    <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -2926,7 +2946,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="28">
+    <row r="5" spans="1:6" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -2946,45 +2966,105 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14">
-      <c r="A6" s="13"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="18"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="13"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="13"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="13"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="13"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="3"/>
+    <row r="6" spans="1:6" ht="13">
+      <c r="A6" s="13">
+        <v>43733</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="16">
+        <v>60</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="13">
+      <c r="A7" s="13">
+        <v>43735</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="16">
+        <v>110</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="13">
+      <c r="A8" s="13">
+        <v>43742</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="16">
+        <v>60</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="13">
+      <c r="A9" s="13">
+        <v>43743</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0</v>
+      </c>
+      <c r="E9" s="16">
+        <v>60</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="13">
+      <c r="A10" s="13">
+        <v>43744</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+      <c r="E10" s="16">
+        <v>240</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="14"/>
@@ -3042,7 +3122,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="14">
+    <row r="18" spans="1:6" ht="13">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3066,7 +3146,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="14">
+    <row r="21" spans="1:6" ht="13">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3229,13 +3309,13 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="42.5" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="42.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -3252,7 +3332,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="16">
+    <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -3270,7 +3350,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="28">
+    <row r="5" spans="1:6" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3290,7 +3370,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15">
+    <row r="6" spans="1:6" ht="16">
       <c r="A6" s="13" t="s">
         <v>16</v>
       </c>
@@ -3308,7 +3388,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15">
+    <row r="7" spans="1:6" ht="16">
       <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
@@ -3326,7 +3406,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15">
+    <row r="8" spans="1:6" ht="16">
       <c r="A8" s="13" t="s">
         <v>30</v>
       </c>
@@ -3344,7 +3424,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15">
+    <row r="9" spans="1:6" ht="16">
       <c r="A9" s="13" t="s">
         <v>31</v>
       </c>
@@ -3380,7 +3460,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15">
+    <row r="11" spans="1:6" ht="16">
       <c r="A11" s="14" t="s">
         <v>33</v>
       </c>
@@ -3446,7 +3526,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="14">
+    <row r="18" spans="1:6" ht="13">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3470,7 +3550,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="14">
+    <row r="21" spans="1:6" ht="13">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3630,16 +3710,16 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="41.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" customWidth="1"/>
+    <col min="6" max="6" width="41.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -3656,7 +3736,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="16">
+    <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -3674,7 +3754,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="28">
+    <row r="5" spans="1:6" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3694,7 +3774,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14">
+    <row r="6" spans="1:6" ht="13">
       <c r="A6" s="13" t="s">
         <v>19</v>
       </c>
@@ -3714,7 +3794,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16">
+    <row r="7" spans="1:6" ht="13">
       <c r="A7" s="13" t="s">
         <v>21</v>
       </c>
@@ -3734,7 +3814,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16">
+    <row r="8" spans="1:6" ht="13">
       <c r="A8" s="13" t="s">
         <v>22</v>
       </c>
@@ -3754,7 +3834,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16">
+    <row r="9" spans="1:6" ht="13">
       <c r="A9" s="13" t="s">
         <v>24</v>
       </c>
@@ -3774,7 +3854,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15">
+    <row r="10" spans="1:6" ht="16">
       <c r="A10" s="13" t="s">
         <v>27</v>
       </c>
@@ -3850,7 +3930,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="14">
+    <row r="18" spans="1:6" ht="13">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3874,7 +3954,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="14">
+    <row r="21" spans="1:6" ht="13">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -4038,13 +4118,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="52.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="52.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4061,7 +4141,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="16">
+    <row r="3" spans="1:7" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -4079,7 +4159,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="28">
+    <row r="5" spans="1:7" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -4099,7 +4179,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14">
+    <row r="6" spans="1:7" ht="13">
       <c r="A6" s="13">
         <v>43733</v>
       </c>
@@ -4219,7 +4299,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="16">
-        <f t="shared" ref="E11:E16" si="1">HOUR(C11)*60+MINUTE(C11)-(HOUR(B11)*60+MINUTE(B11)+D11)</f>
+        <f t="shared" ref="E11:E15" si="1">HOUR(C11)*60+MINUTE(C11)-(HOUR(B11)*60+MINUTE(B11)+D11)</f>
         <v>90</v>
       </c>
       <c r="F11" s="4" t="s">
@@ -4247,7 +4327,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15">
+    <row r="13" spans="1:7" ht="16">
       <c r="A13" s="13">
         <v>43741</v>
       </c>
@@ -4326,7 +4406,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="14">
+    <row r="18" spans="1:6" ht="13">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -4350,7 +4430,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="14">
+    <row r="21" spans="1:6" ht="13">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -4513,13 +4593,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="4" max="4" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="50.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="50.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4536,7 +4616,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="16">
+    <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -4554,7 +4634,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="28">
+    <row r="5" spans="1:6" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -4574,7 +4654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14">
+    <row r="6" spans="1:6" ht="13">
       <c r="A6" s="13"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -4670,7 +4750,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="14">
+    <row r="18" spans="1:6" ht="13">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -4694,7 +4774,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="14">
+    <row r="21" spans="1:6" ht="13">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -4855,7 +4935,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4872,7 +4952,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4889,7 +4969,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
10.13 PMP, PSP(김지환) 수정
</commit_message>
<xml_diff>
--- a/4팀_PSP_Sheet.xlsx
+++ b/4팀_PSP_Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsung\Desktop\강의 등\github\filling good\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\지환\Documents\GitHub\FiillingGood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020FF31B-4ED3-4AB6-9A28-356FBB3E0455}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD13F9C3-6A2E-4A93-936D-CE5E22476277}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2415" yWindow="1635" windowWidth="21150" windowHeight="16530" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="총합" sheetId="1" r:id="rId1"/>
@@ -1480,7 +1480,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="53">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -1832,6 +1832,25 @@
   </si>
   <si>
     <t>usecase outline 수정 및 specification 작성</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.10.13</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UseCase Spec </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>최종 수정, 취합</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2445,16 +2464,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="46.453125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="11.75" customHeight="1">
+    <row r="1" spans="1:6" ht="11.85" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -2466,7 +2485,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="11.75" customHeight="1">
+    <row r="2" spans="1:6" ht="11.85" customHeight="1">
       <c r="A2" s="20"/>
     </row>
     <row r="3" spans="1:6" ht="17.25" customHeight="1">
@@ -2481,8 +2500,8 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:6" ht="11.75" customHeight="1"/>
-    <row r="5" spans="1:6" s="10" customFormat="1" ht="26">
+    <row r="4" spans="1:6" ht="11.85" customHeight="1"/>
+    <row r="5" spans="1:6" s="10" customFormat="1" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -2783,7 +2802,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2800,7 +2819,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2817,7 +2836,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2834,7 +2853,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2851,7 +2870,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2868,7 +2887,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2885,7 +2904,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2901,17 +2920,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="15.453125" customWidth="1"/>
-    <col min="6" max="6" width="49.453125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13">
+    <row r="1" spans="1:6">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -2928,7 +2947,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.5">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -2946,7 +2965,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -2966,7 +2985,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13">
+    <row r="6" spans="1:6">
       <c r="A6" s="13">
         <v>43733</v>
       </c>
@@ -2986,7 +3005,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13">
+    <row r="7" spans="1:6">
       <c r="A7" s="13">
         <v>43735</v>
       </c>
@@ -3006,7 +3025,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13">
+    <row r="8" spans="1:6">
       <c r="A8" s="13">
         <v>43742</v>
       </c>
@@ -3026,7 +3045,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13">
+    <row r="9" spans="1:6">
       <c r="A9" s="13">
         <v>43743</v>
       </c>
@@ -3046,7 +3065,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13">
+    <row r="10" spans="1:6">
       <c r="A10" s="13">
         <v>43744</v>
       </c>
@@ -3122,7 +3141,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13">
+    <row r="18" spans="1:6">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3146,7 +3165,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13">
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3309,13 +3328,13 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="13.453125" customWidth="1"/>
-    <col min="6" max="6" width="42.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13">
+    <row r="1" spans="1:6">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -3332,7 +3351,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.5">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -3350,7 +3369,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3370,7 +3389,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16">
+    <row r="6" spans="1:6" ht="13.5">
       <c r="A6" s="13" t="s">
         <v>16</v>
       </c>
@@ -3388,7 +3407,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16">
+    <row r="7" spans="1:6" ht="13.5">
       <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
@@ -3406,7 +3425,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16">
+    <row r="8" spans="1:6" ht="13.5">
       <c r="A8" s="13" t="s">
         <v>30</v>
       </c>
@@ -3424,7 +3443,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16">
+    <row r="9" spans="1:6" ht="13.5">
       <c r="A9" s="13" t="s">
         <v>31</v>
       </c>
@@ -3460,7 +3479,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16">
+    <row r="11" spans="1:6" ht="13.5">
       <c r="A11" s="14" t="s">
         <v>33</v>
       </c>
@@ -3526,7 +3545,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13">
+    <row r="18" spans="1:6">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3550,7 +3569,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13">
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3709,17 +3728,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="13.81640625" customWidth="1"/>
-    <col min="6" max="6" width="41.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="41.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13">
+    <row r="1" spans="1:6">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -3736,7 +3755,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.5">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -3754,7 +3773,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3774,7 +3793,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13">
+    <row r="6" spans="1:6">
       <c r="A6" s="13" t="s">
         <v>19</v>
       </c>
@@ -3794,7 +3813,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13">
+    <row r="7" spans="1:6" ht="15">
       <c r="A7" s="13" t="s">
         <v>21</v>
       </c>
@@ -3814,7 +3833,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8" s="13" t="s">
         <v>22</v>
       </c>
@@ -3834,7 +3853,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13">
+    <row r="9" spans="1:6" ht="15">
       <c r="A9" s="13" t="s">
         <v>24</v>
       </c>
@@ -3854,7 +3873,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16">
+    <row r="10" spans="1:6" ht="13.5">
       <c r="A10" s="13" t="s">
         <v>27</v>
       </c>
@@ -3874,13 +3893,25 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="14"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="4"/>
+    <row r="11" spans="1:6" ht="15">
+      <c r="A11" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.68402777777777779</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="17">
+        <v>25</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="13"/>
@@ -3930,7 +3961,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13">
+    <row r="18" spans="1:6">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3954,7 +3985,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13">
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -4118,13 +4149,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="52.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="52.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13">
+    <row r="1" spans="1:7">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4141,7 +4172,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="13.5">
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -4159,7 +4190,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="26">
+    <row r="5" spans="1:7" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -4179,7 +4210,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="13">
+    <row r="6" spans="1:7">
       <c r="A6" s="13">
         <v>43733</v>
       </c>
@@ -4327,7 +4358,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16">
+    <row r="13" spans="1:7" ht="13.5">
       <c r="A13" s="13">
         <v>43741</v>
       </c>
@@ -4406,7 +4437,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13">
+    <row r="18" spans="1:6">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -4430,7 +4461,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13">
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -4593,13 +4624,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="11.453125" customWidth="1"/>
-    <col min="6" max="6" width="50.6328125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="50.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13">
+    <row r="1" spans="1:6">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4616,7 +4647,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.5">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -4634,7 +4665,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -4654,7 +4685,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13">
+    <row r="6" spans="1:6">
       <c r="A6" s="13"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -4750,7 +4781,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13">
+    <row r="18" spans="1:6">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -4774,7 +4805,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13">
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -4935,7 +4966,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4952,7 +4983,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4969,7 +5000,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
11.06 PSP(김지환, 함형우), PMP 수정
</commit_message>
<xml_diff>
--- a/4팀_PSP_Sheet.xlsx
+++ b/4팀_PSP_Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\김지현\filling-good\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\지환\Documents\GitHub\FiillingGood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576236AA-1A93-4416-9CDF-85F8D7E4D9C5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306A1BFD-85D7-4EEA-9820-44AD68FC8D6D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9360" yWindow="3210" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="총합" sheetId="1" r:id="rId1"/>
@@ -1480,7 +1480,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="75">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -1954,6 +1954,294 @@
   </si>
   <si>
     <t>19.10.03</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.09.25</t>
+  </si>
+  <si>
+    <t>UseCase Diagram 작성</t>
+  </si>
+  <si>
+    <t>19.09.27</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UseCase Outline </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>토의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>및</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>각</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기능별</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>역할</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>분담</t>
+    </r>
+  </si>
+  <si>
+    <t>19.09.29</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UseCase Outline </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>담당</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>파트</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성</t>
+    </r>
+  </si>
+  <si>
+    <t>19.10.04</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UseCase Spec </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>관련</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>토의</t>
+    </r>
+  </si>
+  <si>
+    <t>19.10.06</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UseCase Spec </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>담당부분</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>19.11.06</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Class Diagram </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2569,13 +2857,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="46.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="11.85" customHeight="1">
@@ -2606,7 +2894,7 @@
       <c r="E3"/>
     </row>
     <row r="4" spans="1:6" ht="11.85" customHeight="1"/>
-    <row r="5" spans="1:6" s="10" customFormat="1" ht="26.4">
+    <row r="5" spans="1:6" s="10" customFormat="1" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -2907,7 +3195,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2924,7 +3212,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2941,7 +3229,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2958,7 +3246,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2975,7 +3263,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2992,7 +3280,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3009,7 +3297,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3029,11 +3317,11 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="49.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3053,7 +3341,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -3071,7 +3359,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3091,7 +3379,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6">
       <c r="A6" s="13">
         <v>43733</v>
       </c>
@@ -3111,7 +3399,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.8">
+    <row r="7" spans="1:6">
       <c r="A7" s="13">
         <v>43735</v>
       </c>
@@ -3131,7 +3419,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.8">
+    <row r="8" spans="1:6">
       <c r="A8" s="13">
         <v>43742</v>
       </c>
@@ -3151,7 +3439,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.8">
+    <row r="9" spans="1:6">
       <c r="A9" s="13">
         <v>43743</v>
       </c>
@@ -3171,7 +3459,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.8">
+    <row r="10" spans="1:6">
       <c r="A10" s="13">
         <v>43744</v>
       </c>
@@ -3259,7 +3547,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3283,7 +3571,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3442,14 +3730,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="42.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3469,7 +3757,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -3487,7 +3775,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3507,7 +3795,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.6">
+    <row r="6" spans="1:6" ht="13.5">
       <c r="A6" s="13" t="s">
         <v>16</v>
       </c>
@@ -3527,7 +3815,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.6">
+    <row r="7" spans="1:6" ht="13.5">
       <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
@@ -3547,7 +3835,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.6">
+    <row r="8" spans="1:6" ht="13.5">
       <c r="A8" s="13" t="s">
         <v>15</v>
       </c>
@@ -3567,7 +3855,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.6">
+    <row r="9" spans="1:6" ht="13.5">
       <c r="A9" s="13" t="s">
         <v>60</v>
       </c>
@@ -3587,7 +3875,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.6">
+    <row r="10" spans="1:6" ht="13.5">
       <c r="A10" s="13" t="s">
         <v>62</v>
       </c>
@@ -3608,7 +3896,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6">
+    <row r="11" spans="1:6" ht="13.5">
       <c r="A11" s="13" t="s">
         <v>23</v>
       </c>
@@ -3648,7 +3936,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.6">
+    <row r="13" spans="1:6" ht="13.5">
       <c r="A13" s="14" t="s">
         <v>30</v>
       </c>
@@ -3668,7 +3956,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6">
+    <row r="14" spans="1:6" ht="13.5">
       <c r="A14" s="13" t="s">
         <v>53</v>
       </c>
@@ -3688,7 +3976,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.6">
+    <row r="15" spans="1:6" ht="13.5">
       <c r="A15" s="13" t="s">
         <v>48</v>
       </c>
@@ -3708,7 +3996,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6">
+    <row r="16" spans="1:6" ht="13.5">
       <c r="A16" s="13" t="s">
         <v>56</v>
       </c>
@@ -3748,7 +4036,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3772,7 +4060,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3931,14 +4219,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="6" max="6" width="41.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="41.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3958,7 +4247,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -3976,7 +4265,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3996,7 +4285,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6">
       <c r="A6" s="13" t="s">
         <v>18</v>
       </c>
@@ -4016,7 +4305,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.8">
+    <row r="7" spans="1:6" ht="15">
       <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
@@ -4036,7 +4325,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.8">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8" s="13" t="s">
         <v>21</v>
       </c>
@@ -4056,7 +4345,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.8">
+    <row r="9" spans="1:6" ht="15">
       <c r="A9" s="13" t="s">
         <v>23</v>
       </c>
@@ -4076,7 +4365,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.6">
+    <row r="10" spans="1:6" ht="13.5">
       <c r="A10" s="13" t="s">
         <v>26</v>
       </c>
@@ -4096,7 +4385,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.8">
+    <row r="11" spans="1:6" ht="15">
       <c r="A11" s="14" t="s">
         <v>48</v>
       </c>
@@ -4116,7 +4405,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.8">
+    <row r="12" spans="1:6" ht="15">
       <c r="A12" s="13" t="s">
         <v>50</v>
       </c>
@@ -4137,13 +4426,25 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="13"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="3"/>
+    <row r="13" spans="1:6" ht="15">
+      <c r="A13" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0</v>
+      </c>
+      <c r="E13" s="16">
+        <v>30</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="13"/>
@@ -4177,7 +4478,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -4201,7 +4502,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -4365,10 +4666,10 @@
       <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
-    <col min="6" max="6" width="52.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="52.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -4388,7 +4689,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="13.8">
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -4406,7 +4707,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="26.4">
+    <row r="5" spans="1:7" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -4426,7 +4727,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="13.8">
+    <row r="6" spans="1:7">
       <c r="A6" s="13">
         <v>43733</v>
       </c>
@@ -4574,7 +4875,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.6">
+    <row r="13" spans="1:7" ht="13.5">
       <c r="A13" s="13">
         <v>43741</v>
       </c>
@@ -4653,7 +4954,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -4677,7 +4978,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -4837,13 +5138,13 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="50.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4863,7 +5164,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -4881,7 +5182,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -4901,61 +5202,145 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
-      <c r="A6" s="13"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="18"/>
+    <row r="6" spans="1:6">
+      <c r="A6" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="16">
+        <v>40</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="13"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="3"/>
+      <c r="A7" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="16">
+        <v>110</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="13"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="3"/>
+      <c r="A8" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="15">
+        <v>60</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="13"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="3"/>
+      <c r="A9" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.73263888888888884</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0</v>
+      </c>
+      <c r="E9" s="16">
+        <v>60</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="13"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="14"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="4"/>
+      <c r="A10" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+      <c r="E10" s="16">
+        <v>120</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="13.5">
+      <c r="A11" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="17">
+        <v>130</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="13"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="3"/>
+      <c r="A12" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="16">
+        <v>60</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="13"/>
@@ -4997,7 +5382,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -5021,7 +5406,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -5182,7 +5567,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5199,7 +5584,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5216,7 +5601,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
11.06 PSP(김지환), PMP 수정
</commit_message>
<xml_diff>
--- a/4팀_PSP_Sheet.xlsx
+++ b/4팀_PSP_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\지환\Documents\GitHub\FiillingGood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306A1BFD-85D7-4EEA-9820-44AD68FC8D6D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0695D85D-C896-422C-B25E-A42E0DF9D62E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="3210" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5430" yWindow="2685" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="총합" sheetId="1" r:id="rId1"/>
@@ -1480,7 +1480,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="77">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -2232,6 +2232,25 @@
   <si>
     <r>
       <t xml:space="preserve">Class Diagram </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.11.06</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ER Diagram </t>
     </r>
     <r>
       <rPr>
@@ -4220,7 +4239,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
@@ -4446,13 +4465,25 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="13"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="3"/>
+    <row r="14" spans="1:6" ht="15">
+      <c r="A14" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0</v>
+      </c>
+      <c r="E14" s="16">
+        <v>40</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="13"/>

</xml_diff>

<commit_message>
11.13 PSP(김지환), PMP 수정
</commit_message>
<xml_diff>
--- a/4팀_PSP_Sheet.xlsx
+++ b/4팀_PSP_Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\김지현\filling-good\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\지환\Documents\GitHub\FiillingGood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CA6232-8D9C-4247-A7DB-59F626C96529}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3614A816-A753-4914-8DDF-169EE62AD793}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15105" yWindow="3675" windowWidth="20310" windowHeight="16110" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="총합" sheetId="1" r:id="rId1"/>
@@ -1480,7 +1480,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="104">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -2465,10 +2465,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Android Studio weekview calendar 공부 및 gui 구성</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>Initial Dataset 수정</t>
     </r>
@@ -2552,6 +2548,176 @@
   </si>
   <si>
     <t>Android Studio weekview calendar 공부 및 GUI 구성</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.11.13</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ERD </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정 및 각 column 정의 문서 작성</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">class diagram, table diagram </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>및</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>관련</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>설명</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>문서</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. SAD </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>발표</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>자료</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3192,13 +3358,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="46.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="11.85" customHeight="1">
@@ -3229,7 +3395,7 @@
       <c r="E3"/>
     </row>
     <row r="4" spans="1:6" ht="11.85" customHeight="1"/>
-    <row r="5" spans="1:6" s="10" customFormat="1" ht="26.4">
+    <row r="5" spans="1:6" s="10" customFormat="1" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3530,7 +3696,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3547,7 +3713,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3564,7 +3730,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3581,7 +3747,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3598,7 +3764,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3615,7 +3781,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3632,7 +3798,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3652,11 +3818,11 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="49.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3676,7 +3842,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -3694,7 +3860,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3714,7 +3880,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6">
       <c r="A6" s="13">
         <v>43733</v>
       </c>
@@ -3734,7 +3900,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.8">
+    <row r="7" spans="1:6">
       <c r="A7" s="13">
         <v>43735</v>
       </c>
@@ -3754,7 +3920,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.8">
+    <row r="8" spans="1:6">
       <c r="A8" s="13">
         <v>43742</v>
       </c>
@@ -3774,7 +3940,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.8">
+    <row r="9" spans="1:6">
       <c r="A9" s="13">
         <v>43743</v>
       </c>
@@ -3794,7 +3960,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.8">
+    <row r="10" spans="1:6">
       <c r="A10" s="13">
         <v>43744</v>
       </c>
@@ -3854,7 +4020,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.8">
+    <row r="13" spans="1:6">
       <c r="A13" s="13">
         <v>43776</v>
       </c>
@@ -3874,7 +4040,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6">
+    <row r="14" spans="1:6" ht="13.5">
       <c r="A14" s="13">
         <v>43778</v>
       </c>
@@ -3891,10 +4057,10 @@
         <v>60</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.6">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="13.5">
       <c r="A15" s="13">
         <v>43781</v>
       </c>
@@ -3911,7 +4077,7 @@
         <v>60</v>
       </c>
       <c r="F15" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3930,7 +4096,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3954,7 +4120,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -4113,14 +4279,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="42.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4140,7 +4306,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -4158,7 +4324,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -4178,7 +4344,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.6">
+    <row r="6" spans="1:6" ht="13.5">
       <c r="A6" s="13" t="s">
         <v>16</v>
       </c>
@@ -4198,7 +4364,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.6">
+    <row r="7" spans="1:6" ht="13.5">
       <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
@@ -4218,7 +4384,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.6">
+    <row r="8" spans="1:6" ht="13.5">
       <c r="A8" s="13" t="s">
         <v>15</v>
       </c>
@@ -4238,7 +4404,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.6">
+    <row r="9" spans="1:6" ht="13.5">
       <c r="A9" s="13" t="s">
         <v>60</v>
       </c>
@@ -4258,7 +4424,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.6">
+    <row r="10" spans="1:6" ht="13.5">
       <c r="A10" s="13" t="s">
         <v>62</v>
       </c>
@@ -4279,7 +4445,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6">
+    <row r="11" spans="1:6" ht="13.5">
       <c r="A11" s="13" t="s">
         <v>23</v>
       </c>
@@ -4319,7 +4485,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.6">
+    <row r="13" spans="1:6" ht="13.5">
       <c r="A13" s="14" t="s">
         <v>30</v>
       </c>
@@ -4339,7 +4505,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6">
+    <row r="14" spans="1:6" ht="13.5">
       <c r="A14" s="13" t="s">
         <v>53</v>
       </c>
@@ -4359,7 +4525,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.6">
+    <row r="15" spans="1:6" ht="13.5">
       <c r="A15" s="13" t="s">
         <v>48</v>
       </c>
@@ -4379,7 +4545,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6">
+    <row r="16" spans="1:6" ht="13.5">
       <c r="A16" s="13" t="s">
         <v>56</v>
       </c>
@@ -4439,7 +4605,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.6">
+    <row r="19" spans="1:6" ht="13.5">
       <c r="A19" s="13" t="s">
         <v>81</v>
       </c>
@@ -4459,7 +4625,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.6">
+    <row r="20" spans="1:6" ht="13.5">
       <c r="A20" s="13" t="s">
         <v>83</v>
       </c>
@@ -4479,7 +4645,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.6">
+    <row r="21" spans="1:6" ht="13.5">
       <c r="A21" s="13" t="s">
         <v>85</v>
       </c>
@@ -4499,7 +4665,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="28.8">
+    <row r="22" spans="1:6" ht="26.25">
       <c r="A22" s="13" t="s">
         <v>92</v>
       </c>
@@ -4519,7 +4685,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.6">
+    <row r="23" spans="1:6" ht="13.5">
       <c r="A23" s="13" t="s">
         <v>94</v>
       </c>
@@ -4536,12 +4702,12 @@
         <v>120</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="13.5">
       <c r="A24" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B24" s="2">
         <v>0</v>
@@ -4556,12 +4722,12 @@
         <v>40</v>
       </c>
       <c r="F24" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B25" s="2">
         <v>4.1666666666666664E-2</v>
@@ -4576,7 +4742,7 @@
         <v>60</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -4698,15 +4864,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="41.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="41.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4726,7 +4892,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -4744,7 +4910,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -4764,7 +4930,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6">
       <c r="A6" s="13" t="s">
         <v>18</v>
       </c>
@@ -4784,7 +4950,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.8">
+    <row r="7" spans="1:6" ht="15">
       <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
@@ -4804,7 +4970,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.8">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8" s="13" t="s">
         <v>21</v>
       </c>
@@ -4824,7 +4990,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.8">
+    <row r="9" spans="1:6" ht="15">
       <c r="A9" s="13" t="s">
         <v>23</v>
       </c>
@@ -4844,7 +5010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.6">
+    <row r="10" spans="1:6" ht="13.5">
       <c r="A10" s="13" t="s">
         <v>26</v>
       </c>
@@ -4864,7 +5030,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.8">
+    <row r="11" spans="1:6" ht="15">
       <c r="A11" s="14" t="s">
         <v>48</v>
       </c>
@@ -4884,7 +5050,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.8">
+    <row r="12" spans="1:6" ht="15">
       <c r="A12" s="13" t="s">
         <v>50</v>
       </c>
@@ -4905,7 +5071,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.8">
+    <row r="13" spans="1:6" ht="15">
       <c r="A13" s="13" t="s">
         <v>73</v>
       </c>
@@ -4925,7 +5091,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.8">
+    <row r="14" spans="1:6" ht="15">
       <c r="A14" s="13" t="s">
         <v>75</v>
       </c>
@@ -4945,7 +5111,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.8">
+    <row r="15" spans="1:6">
       <c r="A15" s="13" t="s">
         <v>87</v>
       </c>
@@ -4965,7 +5131,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13.8">
+    <row r="16" spans="1:6" ht="15">
       <c r="A16" s="13" t="s">
         <v>87</v>
       </c>
@@ -4985,7 +5151,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.8">
+    <row r="17" spans="1:6" ht="15">
       <c r="A17" s="13" t="s">
         <v>87</v>
       </c>
@@ -5005,7 +5171,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6" ht="15">
       <c r="A18" s="13" t="s">
         <v>87</v>
       </c>
@@ -5025,23 +5191,48 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="13"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="13"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="19" spans="1:6" ht="15">
+      <c r="A19" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="D19" s="8">
+        <v>0</v>
+      </c>
+      <c r="E19" s="16">
+        <v>40</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15">
+      <c r="A20" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.96875</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0</v>
+      </c>
+      <c r="E20" s="16">
+        <f>HOUR(C20)*60+MINUTE(C20)-(HOUR(B20)*60+MINUTE(B20)+D20)</f>
+        <v>105</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -5202,13 +5393,13 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="52.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="52.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -5228,7 +5419,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="13.8">
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -5246,7 +5437,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="26.4">
+    <row r="5" spans="1:7" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -5266,7 +5457,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="13.8">
+    <row r="6" spans="1:7">
       <c r="A6" s="13">
         <v>43733</v>
       </c>
@@ -5414,7 +5605,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.6">
+    <row r="13" spans="1:7" ht="13.5">
       <c r="A13" s="13">
         <v>43741</v>
       </c>
@@ -5493,7 +5684,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -5517,7 +5708,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -5680,10 +5871,10 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="50.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -5703,7 +5894,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -5721,7 +5912,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -5741,7 +5932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6">
       <c r="A6" s="13" t="s">
         <v>63</v>
       </c>
@@ -5761,7 +5952,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.8">
+    <row r="7" spans="1:6">
       <c r="A7" s="13" t="s">
         <v>65</v>
       </c>
@@ -5781,7 +5972,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.8">
+    <row r="8" spans="1:6">
       <c r="A8" s="13" t="s">
         <v>67</v>
       </c>
@@ -5801,7 +5992,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.8">
+    <row r="9" spans="1:6">
       <c r="A9" s="13" t="s">
         <v>69</v>
       </c>
@@ -5821,7 +6012,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.8">
+    <row r="10" spans="1:6">
       <c r="A10" s="13" t="s">
         <v>71</v>
       </c>
@@ -5841,7 +6032,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6">
+    <row r="11" spans="1:6" ht="13.5">
       <c r="A11" s="14" t="s">
         <v>30</v>
       </c>
@@ -5921,7 +6112,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -5945,7 +6136,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -6106,7 +6297,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6123,7 +6314,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6140,7 +6331,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
19. 11. 14 김동욱 PSP 수정
</commit_message>
<xml_diff>
--- a/4팀_PSP_Sheet.xlsx
+++ b/4팀_PSP_Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\지환\Documents\GitHub\FiillingGood\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsung\Desktop\강의 등\github\filling good\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3614A816-A753-4914-8DDF-169EE62AD793}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E1659B-48FD-42C4-BDD1-DC81BE485DDB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15105" yWindow="3675" windowWidth="20310" windowHeight="16110" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="총합" sheetId="1" r:id="rId1"/>
@@ -1480,7 +1480,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="105">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -2717,6 +2717,44 @@
         <charset val="129"/>
       </rPr>
       <t>작성</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>추천</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 시스템 로직 정리 및 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ppt </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">작성 </t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -3358,16 +3396,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="46.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="46.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="11.85" customHeight="1">
+    <row r="1" spans="1:6" ht="11.9" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -3379,7 +3417,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="11.85" customHeight="1">
+    <row r="2" spans="1:6" ht="11.9" customHeight="1">
       <c r="A2" s="20"/>
     </row>
     <row r="3" spans="1:6" ht="17.25" customHeight="1">
@@ -3394,8 +3432,8 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:6" ht="11.85" customHeight="1"/>
-    <row r="5" spans="1:6" s="10" customFormat="1" ht="25.5">
+    <row r="4" spans="1:6" ht="11.9" customHeight="1"/>
+    <row r="5" spans="1:6" s="10" customFormat="1" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3696,7 +3734,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3713,7 +3751,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3730,7 +3768,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3747,7 +3785,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3764,7 +3802,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3781,7 +3819,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3798,7 +3836,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3814,18 +3852,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="49.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" customWidth="1"/>
+    <col min="6" max="6" width="49.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -3842,7 +3880,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -3860,7 +3898,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="25.5">
+    <row r="5" spans="1:6" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3880,7 +3918,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="13">
       <c r="A6" s="13">
         <v>43733</v>
       </c>
@@ -3900,7 +3938,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="13">
       <c r="A7" s="13">
         <v>43735</v>
       </c>
@@ -3920,7 +3958,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="13">
       <c r="A8" s="13">
         <v>43742</v>
       </c>
@@ -3940,7 +3978,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="13">
       <c r="A9" s="13">
         <v>43743</v>
       </c>
@@ -3960,7 +3998,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="13">
       <c r="A10" s="13">
         <v>43744</v>
       </c>
@@ -4020,7 +4058,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="13">
       <c r="A13" s="13">
         <v>43776</v>
       </c>
@@ -4040,7 +4078,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.5">
+    <row r="14" spans="1:6" ht="16">
       <c r="A14" s="13">
         <v>43778</v>
       </c>
@@ -4060,7 +4098,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.5">
+    <row r="15" spans="1:6" ht="16">
       <c r="A15" s="13">
         <v>43781</v>
       </c>
@@ -4080,13 +4118,25 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="13"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="3"/>
+    <row r="16" spans="1:6" ht="16">
+      <c r="A16" s="13">
+        <v>43782</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0</v>
+      </c>
+      <c r="E16" s="16">
+        <v>210</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="13"/>
@@ -4096,7 +4146,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" ht="13">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -4120,7 +4170,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" ht="13">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -4283,13 +4333,13 @@
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="42.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="42.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4306,7 +4356,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -4324,7 +4374,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="25.5">
+    <row r="5" spans="1:6" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -4344,7 +4394,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.5">
+    <row r="6" spans="1:6" ht="16">
       <c r="A6" s="13" t="s">
         <v>16</v>
       </c>
@@ -4364,7 +4414,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.5">
+    <row r="7" spans="1:6" ht="16">
       <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
@@ -4384,7 +4434,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.5">
+    <row r="8" spans="1:6" ht="16">
       <c r="A8" s="13" t="s">
         <v>15</v>
       </c>
@@ -4404,7 +4454,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.5">
+    <row r="9" spans="1:6" ht="16">
       <c r="A9" s="13" t="s">
         <v>60</v>
       </c>
@@ -4424,7 +4474,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.5">
+    <row r="10" spans="1:6" ht="16">
       <c r="A10" s="13" t="s">
         <v>62</v>
       </c>
@@ -4445,7 +4495,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.5">
+    <row r="11" spans="1:6" ht="16">
       <c r="A11" s="13" t="s">
         <v>23</v>
       </c>
@@ -4485,7 +4535,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.5">
+    <row r="13" spans="1:6" ht="16">
       <c r="A13" s="14" t="s">
         <v>30</v>
       </c>
@@ -4505,7 +4555,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.5">
+    <row r="14" spans="1:6" ht="16">
       <c r="A14" s="13" t="s">
         <v>53</v>
       </c>
@@ -4525,7 +4575,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.5">
+    <row r="15" spans="1:6" ht="16">
       <c r="A15" s="13" t="s">
         <v>48</v>
       </c>
@@ -4545,7 +4595,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13.5">
+    <row r="16" spans="1:6" ht="16">
       <c r="A16" s="13" t="s">
         <v>56</v>
       </c>
@@ -4605,7 +4655,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.5">
+    <row r="19" spans="1:6" ht="16">
       <c r="A19" s="13" t="s">
         <v>81</v>
       </c>
@@ -4625,7 +4675,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.5">
+    <row r="20" spans="1:6" ht="16">
       <c r="A20" s="13" t="s">
         <v>83</v>
       </c>
@@ -4645,7 +4695,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.5">
+    <row r="21" spans="1:6" ht="16">
       <c r="A21" s="13" t="s">
         <v>85</v>
       </c>
@@ -4665,7 +4715,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="26.25">
+    <row r="22" spans="1:6" ht="28.5">
       <c r="A22" s="13" t="s">
         <v>92</v>
       </c>
@@ -4685,7 +4735,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="13.5">
+    <row r="23" spans="1:6" ht="16">
       <c r="A23" s="13" t="s">
         <v>94</v>
       </c>
@@ -4705,7 +4755,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="13.5">
+    <row r="24" spans="1:6" ht="16">
       <c r="A24" s="13" t="s">
         <v>97</v>
       </c>
@@ -4864,18 +4914,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="41.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" customWidth="1"/>
+    <col min="6" max="6" width="41.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4892,7 +4942,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -4910,7 +4960,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="25.5">
+    <row r="5" spans="1:6" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -4930,7 +4980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="13">
       <c r="A6" s="13" t="s">
         <v>18</v>
       </c>
@@ -4950,7 +5000,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15">
+    <row r="7" spans="1:6" ht="13">
       <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
@@ -4970,7 +5020,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15">
+    <row r="8" spans="1:6" ht="13">
       <c r="A8" s="13" t="s">
         <v>21</v>
       </c>
@@ -4990,7 +5040,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15">
+    <row r="9" spans="1:6" ht="13">
       <c r="A9" s="13" t="s">
         <v>23</v>
       </c>
@@ -5010,7 +5060,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.5">
+    <row r="10" spans="1:6" ht="16">
       <c r="A10" s="13" t="s">
         <v>26</v>
       </c>
@@ -5030,7 +5080,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15">
+    <row r="11" spans="1:6" ht="13">
       <c r="A11" s="14" t="s">
         <v>48</v>
       </c>
@@ -5050,7 +5100,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15">
+    <row r="12" spans="1:6" ht="13">
       <c r="A12" s="13" t="s">
         <v>50</v>
       </c>
@@ -5071,7 +5121,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15">
+    <row r="13" spans="1:6" ht="13">
       <c r="A13" s="13" t="s">
         <v>73</v>
       </c>
@@ -5091,7 +5141,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15">
+    <row r="14" spans="1:6" ht="13">
       <c r="A14" s="13" t="s">
         <v>75</v>
       </c>
@@ -5111,7 +5161,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="13">
       <c r="A15" s="13" t="s">
         <v>87</v>
       </c>
@@ -5131,7 +5181,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15">
+    <row r="16" spans="1:6" ht="13">
       <c r="A16" s="13" t="s">
         <v>87</v>
       </c>
@@ -5151,7 +5201,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15">
+    <row r="17" spans="1:6" ht="13">
       <c r="A17" s="13" t="s">
         <v>87</v>
       </c>
@@ -5171,7 +5221,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15">
+    <row r="18" spans="1:6" ht="13">
       <c r="A18" s="13" t="s">
         <v>87</v>
       </c>
@@ -5191,7 +5241,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15">
+    <row r="19" spans="1:6" ht="13">
       <c r="A19" s="13" t="s">
         <v>101</v>
       </c>
@@ -5211,7 +5261,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15">
+    <row r="20" spans="1:6" ht="13">
       <c r="A20" s="13" t="s">
         <v>101</v>
       </c>
@@ -5232,7 +5282,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" ht="13">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -5396,13 +5446,13 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" customWidth="1"/>
+    <col min="6" max="6" width="52.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5419,7 +5469,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="15">
+    <row r="3" spans="1:7" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -5437,7 +5487,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="25.5">
+    <row r="5" spans="1:7" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -5457,7 +5507,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="13">
       <c r="A6" s="13">
         <v>43733</v>
       </c>
@@ -5605,7 +5655,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="13.5">
+    <row r="13" spans="1:7" ht="16">
       <c r="A13" s="13">
         <v>43741</v>
       </c>
@@ -5684,7 +5734,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" ht="13">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -5708,7 +5758,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" ht="13">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -5871,13 +5921,13 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="50.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="50.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5894,7 +5944,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -5912,7 +5962,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="25.5">
+    <row r="5" spans="1:6" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -5932,7 +5982,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="13">
       <c r="A6" s="13" t="s">
         <v>63</v>
       </c>
@@ -5952,7 +6002,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="13">
       <c r="A7" s="13" t="s">
         <v>65</v>
       </c>
@@ -5972,7 +6022,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="13">
       <c r="A8" s="13" t="s">
         <v>67</v>
       </c>
@@ -5992,7 +6042,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="13">
       <c r="A9" s="13" t="s">
         <v>69</v>
       </c>
@@ -6012,7 +6062,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="13">
       <c r="A10" s="13" t="s">
         <v>71</v>
       </c>
@@ -6032,7 +6082,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.5">
+    <row r="11" spans="1:6" ht="16">
       <c r="A11" s="14" t="s">
         <v>30</v>
       </c>
@@ -6112,7 +6162,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" ht="13">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -6136,7 +6186,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" ht="13">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -6297,7 +6347,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6314,7 +6364,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6331,7 +6381,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
11.19 PSP(김지환), PMP 수정 및 Spec 1.1 update
</commit_message>
<xml_diff>
--- a/4팀_PSP_Sheet.xlsx
+++ b/4팀_PSP_Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\김지현\filling-good\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\지환\Documents\GitHub\FiillingGood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42BFA20-7DEF-4120-ABCE-7BD42DC2921C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C737228-DEBA-4DB2-8533-84B4508F5F7E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17130" yWindow="2820" windowWidth="20310" windowHeight="16110" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="총합" sheetId="1" r:id="rId1"/>
@@ -1480,7 +1480,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="112">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -2815,6 +2815,14 @@
   </si>
   <si>
     <t>fragment 공부 및 적용, 각종 에러들 해결</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.11.19</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMP 수정 및 Spec Update</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3455,13 +3463,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="46.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="11.85" customHeight="1">
@@ -3492,7 +3500,7 @@
       <c r="E3"/>
     </row>
     <row r="4" spans="1:6" ht="11.85" customHeight="1"/>
-    <row r="5" spans="1:6" s="10" customFormat="1" ht="26.4">
+    <row r="5" spans="1:6" s="10" customFormat="1" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3793,7 +3801,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3810,7 +3818,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3827,7 +3835,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3844,7 +3852,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3861,7 +3869,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3878,7 +3886,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3895,7 +3903,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3915,11 +3923,11 @@
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="49.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3939,7 +3947,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -3957,7 +3965,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3977,7 +3985,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6">
       <c r="A6" s="13">
         <v>43733</v>
       </c>
@@ -3997,7 +4005,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.8">
+    <row r="7" spans="1:6">
       <c r="A7" s="13">
         <v>43735</v>
       </c>
@@ -4017,7 +4025,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.8">
+    <row r="8" spans="1:6">
       <c r="A8" s="13">
         <v>43742</v>
       </c>
@@ -4037,7 +4045,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.8">
+    <row r="9" spans="1:6">
       <c r="A9" s="13">
         <v>43743</v>
       </c>
@@ -4057,7 +4065,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.8">
+    <row r="10" spans="1:6">
       <c r="A10" s="13">
         <v>43744</v>
       </c>
@@ -4117,7 +4125,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.8">
+    <row r="13" spans="1:6">
       <c r="A13" s="13">
         <v>43776</v>
       </c>
@@ -4137,7 +4145,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6">
+    <row r="14" spans="1:6" ht="13.5">
       <c r="A14" s="13">
         <v>43778</v>
       </c>
@@ -4157,7 +4165,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.6">
+    <row r="15" spans="1:6" ht="13.5">
       <c r="A15" s="13">
         <v>43781</v>
       </c>
@@ -4177,7 +4185,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6">
+    <row r="16" spans="1:6" ht="13.5">
       <c r="A16" s="13">
         <v>43782</v>
       </c>
@@ -4205,7 +4213,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -4229,7 +4237,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -4388,14 +4396,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="42.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4415,7 +4423,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -4433,7 +4441,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -4453,7 +4461,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.6">
+    <row r="6" spans="1:6" ht="13.5">
       <c r="A6" s="13" t="s">
         <v>16</v>
       </c>
@@ -4473,7 +4481,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.6">
+    <row r="7" spans="1:6" ht="13.5">
       <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
@@ -4493,7 +4501,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.6">
+    <row r="8" spans="1:6" ht="13.5">
       <c r="A8" s="13" t="s">
         <v>15</v>
       </c>
@@ -4513,7 +4521,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.6">
+    <row r="9" spans="1:6" ht="13.5">
       <c r="A9" s="13" t="s">
         <v>60</v>
       </c>
@@ -4533,7 +4541,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.6">
+    <row r="10" spans="1:6" ht="13.5">
       <c r="A10" s="13" t="s">
         <v>62</v>
       </c>
@@ -4554,7 +4562,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6">
+    <row r="11" spans="1:6" ht="13.5">
       <c r="A11" s="13" t="s">
         <v>23</v>
       </c>
@@ -4594,7 +4602,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.6">
+    <row r="13" spans="1:6" ht="13.5">
       <c r="A13" s="14" t="s">
         <v>30</v>
       </c>
@@ -4614,7 +4622,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6">
+    <row r="14" spans="1:6" ht="13.5">
       <c r="A14" s="13" t="s">
         <v>53</v>
       </c>
@@ -4634,7 +4642,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.6">
+    <row r="15" spans="1:6" ht="13.5">
       <c r="A15" s="13" t="s">
         <v>48</v>
       </c>
@@ -4654,7 +4662,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6">
+    <row r="16" spans="1:6" ht="13.5">
       <c r="A16" s="13" t="s">
         <v>56</v>
       </c>
@@ -4714,7 +4722,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.6">
+    <row r="19" spans="1:6" ht="13.5">
       <c r="A19" s="13" t="s">
         <v>81</v>
       </c>
@@ -4734,7 +4742,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.6">
+    <row r="20" spans="1:6" ht="13.5">
       <c r="A20" s="13" t="s">
         <v>83</v>
       </c>
@@ -4754,7 +4762,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.6">
+    <row r="21" spans="1:6" ht="13.5">
       <c r="A21" s="13" t="s">
         <v>85</v>
       </c>
@@ -4774,7 +4782,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="28.8">
+    <row r="22" spans="1:6" ht="26.25">
       <c r="A22" s="13" t="s">
         <v>92</v>
       </c>
@@ -4794,7 +4802,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.6">
+    <row r="23" spans="1:6" ht="13.5">
       <c r="A23" s="13" t="s">
         <v>94</v>
       </c>
@@ -4814,7 +4822,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.6">
+    <row r="24" spans="1:6" ht="13.5">
       <c r="A24" s="13" t="s">
         <v>97</v>
       </c>
@@ -4834,7 +4842,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.6">
+    <row r="25" spans="1:6" ht="13.5">
       <c r="A25" s="13" t="s">
         <v>97</v>
       </c>
@@ -4854,7 +4862,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.6">
+    <row r="26" spans="1:6" ht="13.5">
       <c r="A26" s="13" t="s">
         <v>104</v>
       </c>
@@ -4874,7 +4882,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.6">
+    <row r="27" spans="1:6" ht="13.5">
       <c r="A27" s="13" t="s">
         <v>104</v>
       </c>
@@ -4894,7 +4902,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.6">
+    <row r="28" spans="1:6" ht="13.5">
       <c r="A28" s="13" t="s">
         <v>108</v>
       </c>
@@ -5009,15 +5017,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" customWidth="1"/>
-    <col min="6" max="6" width="41.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="41.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -5037,7 +5045,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -5055,7 +5063,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -5075,7 +5083,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6">
       <c r="A6" s="13" t="s">
         <v>18</v>
       </c>
@@ -5095,7 +5103,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.8">
+    <row r="7" spans="1:6" ht="15">
       <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
@@ -5115,7 +5123,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.8">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8" s="13" t="s">
         <v>21</v>
       </c>
@@ -5135,7 +5143,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.8">
+    <row r="9" spans="1:6" ht="15">
       <c r="A9" s="13" t="s">
         <v>23</v>
       </c>
@@ -5155,7 +5163,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.6">
+    <row r="10" spans="1:6" ht="13.5">
       <c r="A10" s="13" t="s">
         <v>26</v>
       </c>
@@ -5175,7 +5183,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.8">
+    <row r="11" spans="1:6" ht="15">
       <c r="A11" s="14" t="s">
         <v>48</v>
       </c>
@@ -5195,7 +5203,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.8">
+    <row r="12" spans="1:6" ht="15">
       <c r="A12" s="13" t="s">
         <v>50</v>
       </c>
@@ -5216,7 +5224,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.8">
+    <row r="13" spans="1:6" ht="15">
       <c r="A13" s="13" t="s">
         <v>73</v>
       </c>
@@ -5236,7 +5244,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.8">
+    <row r="14" spans="1:6" ht="15">
       <c r="A14" s="13" t="s">
         <v>75</v>
       </c>
@@ -5256,7 +5264,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.8">
+    <row r="15" spans="1:6">
       <c r="A15" s="13" t="s">
         <v>87</v>
       </c>
@@ -5276,7 +5284,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13.8">
+    <row r="16" spans="1:6" ht="15">
       <c r="A16" s="13" t="s">
         <v>87</v>
       </c>
@@ -5296,7 +5304,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.8">
+    <row r="17" spans="1:6" ht="15">
       <c r="A17" s="13" t="s">
         <v>87</v>
       </c>
@@ -5316,7 +5324,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6" ht="15">
       <c r="A18" s="13" t="s">
         <v>87</v>
       </c>
@@ -5336,7 +5344,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.8">
+    <row r="19" spans="1:6" ht="15">
       <c r="A19" s="13" t="s">
         <v>100</v>
       </c>
@@ -5356,7 +5364,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.8">
+    <row r="20" spans="1:6" ht="15">
       <c r="A20" s="13" t="s">
         <v>100</v>
       </c>
@@ -5377,13 +5385,25 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
-      <c r="A21" s="13"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="18"/>
+    <row r="21" spans="1:6">
+      <c r="A21" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.90277777777777779</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0</v>
+      </c>
+      <c r="E21" s="16">
+        <v>40</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="13"/>
@@ -5541,10 +5561,10 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="52.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="52.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -5564,7 +5584,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="13.8">
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -5582,7 +5602,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="26.4">
+    <row r="5" spans="1:7" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -5602,7 +5622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="13.8">
+    <row r="6" spans="1:7">
       <c r="A6" s="13">
         <v>43733</v>
       </c>
@@ -5750,7 +5770,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.6">
+    <row r="13" spans="1:7" ht="13.5">
       <c r="A13" s="13">
         <v>43741</v>
       </c>
@@ -5829,7 +5849,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -5853,7 +5873,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -6016,10 +6036,10 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="50.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -6039,7 +6059,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -6057,7 +6077,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -6077,7 +6097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6">
       <c r="A6" s="13" t="s">
         <v>63</v>
       </c>
@@ -6097,7 +6117,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.8">
+    <row r="7" spans="1:6">
       <c r="A7" s="13" t="s">
         <v>65</v>
       </c>
@@ -6117,7 +6137,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.8">
+    <row r="8" spans="1:6">
       <c r="A8" s="13" t="s">
         <v>67</v>
       </c>
@@ -6137,7 +6157,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.8">
+    <row r="9" spans="1:6">
       <c r="A9" s="13" t="s">
         <v>69</v>
       </c>
@@ -6157,7 +6177,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.8">
+    <row r="10" spans="1:6">
       <c r="A10" s="13" t="s">
         <v>71</v>
       </c>
@@ -6177,7 +6197,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6">
+    <row r="11" spans="1:6" ht="13.5">
       <c r="A11" s="14" t="s">
         <v>30</v>
       </c>
@@ -6257,7 +6277,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -6281,7 +6301,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -6442,7 +6462,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6459,7 +6479,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6476,7 +6496,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
12.02 PSP(김지환), PMP 수정
</commit_message>
<xml_diff>
--- a/4팀_PSP_Sheet.xlsx
+++ b/4팀_PSP_Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\filling-good\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\지환\Documents\GitHub\FiillingGood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0200566-8D89-4F17-AD08-F56AF9175922}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFA1025-49ED-4465-A4E6-96BBA526DC3A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11775" yWindow="4095" windowWidth="20310" windowHeight="16110" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="총합" sheetId="1" r:id="rId1"/>
@@ -1480,7 +1480,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="139">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -2979,6 +2979,25 @@
   </si>
   <si>
     <t>뒤로 가기 기능, 알림 메시지, 외부 일정 연동 페이지 추가 및 SRS 1.2 수정</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.12.02</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">php - Mysql </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>연동 구축</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3623,13 +3642,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="46.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="11.85" customHeight="1">
@@ -3660,7 +3679,7 @@
       <c r="E3"/>
     </row>
     <row r="4" spans="1:6" ht="11.85" customHeight="1"/>
-    <row r="5" spans="1:6" s="10" customFormat="1" ht="26.4">
+    <row r="5" spans="1:6" s="10" customFormat="1" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3961,7 +3980,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3978,7 +3997,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3995,7 +4014,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4012,7 +4031,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4029,7 +4048,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4046,7 +4065,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4063,7 +4082,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4083,11 +4102,11 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="49.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4107,7 +4126,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -4125,7 +4144,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -4145,7 +4164,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6">
       <c r="A6" s="13">
         <v>43733</v>
       </c>
@@ -4165,7 +4184,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.8">
+    <row r="7" spans="1:6">
       <c r="A7" s="13">
         <v>43735</v>
       </c>
@@ -4185,7 +4204,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.8">
+    <row r="8" spans="1:6">
       <c r="A8" s="13">
         <v>43742</v>
       </c>
@@ -4205,7 +4224,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.8">
+    <row r="9" spans="1:6">
       <c r="A9" s="13">
         <v>43743</v>
       </c>
@@ -4225,7 +4244,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.8">
+    <row r="10" spans="1:6">
       <c r="A10" s="13">
         <v>43744</v>
       </c>
@@ -4285,7 +4304,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.8">
+    <row r="13" spans="1:6">
       <c r="A13" s="13">
         <v>43776</v>
       </c>
@@ -4305,7 +4324,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6">
+    <row r="14" spans="1:6" ht="13.5">
       <c r="A14" s="13">
         <v>43778</v>
       </c>
@@ -4325,7 +4344,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.6">
+    <row r="15" spans="1:6" ht="13.5">
       <c r="A15" s="13">
         <v>43781</v>
       </c>
@@ -4345,7 +4364,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6">
+    <row r="16" spans="1:6" ht="13.5">
       <c r="A16" s="13">
         <v>43782</v>
       </c>
@@ -4365,7 +4384,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.6">
+    <row r="17" spans="1:6" ht="13.5">
       <c r="A17" s="13">
         <v>43791</v>
       </c>
@@ -4385,7 +4404,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6">
       <c r="A18" s="13">
         <v>43792</v>
       </c>
@@ -4405,7 +4424,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.8">
+    <row r="19" spans="1:6">
       <c r="A19" s="13">
         <v>43793</v>
       </c>
@@ -4425,7 +4444,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.8">
+    <row r="20" spans="1:6">
       <c r="A20" s="13">
         <v>43794</v>
       </c>
@@ -4445,7 +4464,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6">
       <c r="A21" s="13">
         <v>43795</v>
       </c>
@@ -4616,15 +4635,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="42.44140625" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4644,7 +4663,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -4662,7 +4681,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -4682,7 +4701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.6">
+    <row r="6" spans="1:6" ht="13.5">
       <c r="A6" s="13" t="s">
         <v>16</v>
       </c>
@@ -4702,7 +4721,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.6">
+    <row r="7" spans="1:6" ht="13.5">
       <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
@@ -4722,7 +4741,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.6">
+    <row r="8" spans="1:6" ht="13.5">
       <c r="A8" s="13" t="s">
         <v>15</v>
       </c>
@@ -4742,7 +4761,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.6">
+    <row r="9" spans="1:6" ht="13.5">
       <c r="A9" s="13" t="s">
         <v>60</v>
       </c>
@@ -4762,7 +4781,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.6">
+    <row r="10" spans="1:6" ht="13.5">
       <c r="A10" s="13" t="s">
         <v>62</v>
       </c>
@@ -4783,7 +4802,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6">
+    <row r="11" spans="1:6" ht="13.5">
       <c r="A11" s="13" t="s">
         <v>23</v>
       </c>
@@ -4823,7 +4842,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.6">
+    <row r="13" spans="1:6" ht="13.5">
       <c r="A13" s="14" t="s">
         <v>30</v>
       </c>
@@ -4843,7 +4862,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6">
+    <row r="14" spans="1:6" ht="13.5">
       <c r="A14" s="13" t="s">
         <v>53</v>
       </c>
@@ -4863,7 +4882,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.6">
+    <row r="15" spans="1:6" ht="13.5">
       <c r="A15" s="13" t="s">
         <v>48</v>
       </c>
@@ -4883,7 +4902,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6">
+    <row r="16" spans="1:6" ht="13.5">
       <c r="A16" s="13" t="s">
         <v>56</v>
       </c>
@@ -4943,7 +4962,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.6">
+    <row r="19" spans="1:6" ht="13.5">
       <c r="A19" s="13" t="s">
         <v>81</v>
       </c>
@@ -4963,7 +4982,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.6">
+    <row r="20" spans="1:6" ht="13.5">
       <c r="A20" s="13" t="s">
         <v>83</v>
       </c>
@@ -4983,7 +5002,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.6">
+    <row r="21" spans="1:6" ht="13.5">
       <c r="A21" s="13" t="s">
         <v>85</v>
       </c>
@@ -5003,7 +5022,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="28.8">
+    <row r="22" spans="1:6" ht="26.25">
       <c r="A22" s="13" t="s">
         <v>92</v>
       </c>
@@ -5023,7 +5042,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.6">
+    <row r="23" spans="1:6" ht="13.5">
       <c r="A23" s="13" t="s">
         <v>94</v>
       </c>
@@ -5043,7 +5062,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.6">
+    <row r="24" spans="1:6" ht="13.5">
       <c r="A24" s="13" t="s">
         <v>97</v>
       </c>
@@ -5063,7 +5082,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.6">
+    <row r="25" spans="1:6" ht="13.5">
       <c r="A25" s="13" t="s">
         <v>97</v>
       </c>
@@ -5083,7 +5102,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.6">
+    <row r="26" spans="1:6" ht="13.5">
       <c r="A26" s="13" t="s">
         <v>104</v>
       </c>
@@ -5103,7 +5122,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.6">
+    <row r="27" spans="1:6" ht="13.5">
       <c r="A27" s="13" t="s">
         <v>104</v>
       </c>
@@ -5123,7 +5142,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.6">
+    <row r="28" spans="1:6" ht="13.5">
       <c r="A28" s="13" t="s">
         <v>108</v>
       </c>
@@ -5143,7 +5162,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.6">
+    <row r="29" spans="1:6" ht="13.5">
       <c r="A29" s="13" t="s">
         <v>114</v>
       </c>
@@ -5163,7 +5182,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.6">
+    <row r="30" spans="1:6" ht="13.5">
       <c r="A30" s="13" t="s">
         <v>115</v>
       </c>
@@ -5243,7 +5262,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.6">
+    <row r="34" spans="1:6" ht="13.5">
       <c r="A34" s="13" t="s">
         <v>121</v>
       </c>
@@ -5263,7 +5282,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.6">
+    <row r="35" spans="1:6" ht="13.5">
       <c r="A35" s="13" t="s">
         <v>123</v>
       </c>
@@ -5283,7 +5302,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="31.2">
+    <row r="36" spans="1:6" ht="27">
       <c r="A36" s="13" t="s">
         <v>135</v>
       </c>
@@ -5334,15 +5353,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="41.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="41.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -5362,7 +5381,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -5380,7 +5399,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -5400,7 +5419,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6">
       <c r="A6" s="13" t="s">
         <v>18</v>
       </c>
@@ -5420,7 +5439,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.8">
+    <row r="7" spans="1:6" ht="15">
       <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
@@ -5440,7 +5459,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.8">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8" s="13" t="s">
         <v>21</v>
       </c>
@@ -5460,7 +5479,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.8">
+    <row r="9" spans="1:6" ht="15">
       <c r="A9" s="13" t="s">
         <v>23</v>
       </c>
@@ -5480,7 +5499,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.6">
+    <row r="10" spans="1:6" ht="13.5">
       <c r="A10" s="13" t="s">
         <v>26</v>
       </c>
@@ -5500,7 +5519,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.8">
+    <row r="11" spans="1:6" ht="15">
       <c r="A11" s="14" t="s">
         <v>48</v>
       </c>
@@ -5520,7 +5539,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.8">
+    <row r="12" spans="1:6" ht="15">
       <c r="A12" s="13" t="s">
         <v>50</v>
       </c>
@@ -5541,7 +5560,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.8">
+    <row r="13" spans="1:6" ht="15">
       <c r="A13" s="13" t="s">
         <v>73</v>
       </c>
@@ -5561,7 +5580,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.8">
+    <row r="14" spans="1:6" ht="15">
       <c r="A14" s="13" t="s">
         <v>75</v>
       </c>
@@ -5581,7 +5600,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.8">
+    <row r="15" spans="1:6">
       <c r="A15" s="13" t="s">
         <v>87</v>
       </c>
@@ -5601,7 +5620,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13.8">
+    <row r="16" spans="1:6" ht="15">
       <c r="A16" s="13" t="s">
         <v>87</v>
       </c>
@@ -5621,7 +5640,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.8">
+    <row r="17" spans="1:6" ht="15">
       <c r="A17" s="13" t="s">
         <v>87</v>
       </c>
@@ -5641,7 +5660,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6" ht="15">
       <c r="A18" s="13" t="s">
         <v>87</v>
       </c>
@@ -5661,7 +5680,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.8">
+    <row r="19" spans="1:6" ht="15">
       <c r="A19" s="13" t="s">
         <v>100</v>
       </c>
@@ -5681,7 +5700,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.8">
+    <row r="20" spans="1:6" ht="15">
       <c r="A20" s="13" t="s">
         <v>100</v>
       </c>
@@ -5702,7 +5721,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6">
       <c r="A21" s="13" t="s">
         <v>110</v>
       </c>
@@ -5722,7 +5741,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.8">
+    <row r="22" spans="1:6" ht="15">
       <c r="A22" s="13" t="s">
         <v>112</v>
       </c>
@@ -5743,7 +5762,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="13.8">
+    <row r="23" spans="1:6" ht="15">
       <c r="A23" s="13" t="s">
         <v>128</v>
       </c>
@@ -5763,7 +5782,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="13.8">
+    <row r="24" spans="1:6" ht="15">
       <c r="A24" s="13" t="s">
         <v>130</v>
       </c>
@@ -5783,7 +5802,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="13.8">
+    <row r="25" spans="1:6" ht="15">
       <c r="A25" s="13" t="s">
         <v>130</v>
       </c>
@@ -5803,7 +5822,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="13.8">
+    <row r="26" spans="1:6" ht="15">
       <c r="A26" s="13" t="s">
         <v>133</v>
       </c>
@@ -5823,13 +5842,25 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="13"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="3"/>
+    <row r="27" spans="1:6" ht="15">
+      <c r="A27" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="D27" s="8">
+        <v>0</v>
+      </c>
+      <c r="E27" s="16">
+        <v>140</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="13"/>
@@ -5939,10 +5970,10 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="52.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="52.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -5962,7 +5993,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="13.8">
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -5980,7 +6011,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="26.4">
+    <row r="5" spans="1:7" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -6000,7 +6031,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="13.8">
+    <row r="6" spans="1:7">
       <c r="A6" s="13">
         <v>43733</v>
       </c>
@@ -6148,7 +6179,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.6">
+    <row r="13" spans="1:7" ht="13.5">
       <c r="A13" s="13">
         <v>43741</v>
       </c>
@@ -6227,7 +6258,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -6251,7 +6282,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -6414,10 +6445,10 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="50.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -6437,7 +6468,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -6455,7 +6486,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -6475,7 +6506,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6">
       <c r="A6" s="13" t="s">
         <v>63</v>
       </c>
@@ -6495,7 +6526,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.8">
+    <row r="7" spans="1:6">
       <c r="A7" s="13" t="s">
         <v>65</v>
       </c>
@@ -6515,7 +6546,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.8">
+    <row r="8" spans="1:6">
       <c r="A8" s="13" t="s">
         <v>67</v>
       </c>
@@ -6535,7 +6566,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.8">
+    <row r="9" spans="1:6">
       <c r="A9" s="13" t="s">
         <v>69</v>
       </c>
@@ -6555,7 +6586,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.8">
+    <row r="10" spans="1:6">
       <c r="A10" s="13" t="s">
         <v>71</v>
       </c>
@@ -6575,7 +6606,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6">
+    <row r="11" spans="1:6" ht="13.5">
       <c r="A11" s="14" t="s">
         <v>30</v>
       </c>
@@ -6655,7 +6686,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -6679,7 +6710,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -6840,7 +6871,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6857,7 +6888,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6874,7 +6905,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
12.04 PSP(김지환), SRS 수정
</commit_message>
<xml_diff>
--- a/4팀_PSP_Sheet.xlsx
+++ b/4팀_PSP_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\지환\Documents\GitHub\FiillingGood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE97F84-8397-429E-9EFB-05B9A74D4A62}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41FD7EA-10EC-4A9F-A8A1-BB34F89301D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1480,7 +1480,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="143">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -3030,6 +3030,42 @@
         <charset val="129"/>
       </rPr>
       <t>연동 구현</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.12.04</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">DB boundary </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">함수 구현, 실제 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">DB </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>구축</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -5915,13 +5951,25 @@
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="13"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="3"/>
+    <row r="29" spans="1:6" ht="15">
+      <c r="A29" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D29" s="8">
+        <v>20</v>
+      </c>
+      <c r="E29" s="16">
+        <v>190</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="13"/>

</xml_diff>

<commit_message>
12.05 PSP(김지환, 함형우) 수정, SRS 수정, TestCase 수정
</commit_message>
<xml_diff>
--- a/4팀_PSP_Sheet.xlsx
+++ b/4팀_PSP_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\지환\Documents\GitHub\FiillingGood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41FD7EA-10EC-4A9F-A8A1-BB34F89301D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8224C33D-EE27-4A94-8D71-434C77C66D78}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1605" yWindow="3060" windowWidth="20310" windowHeight="16110" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="총합" sheetId="1" r:id="rId1"/>
@@ -1480,7 +1480,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="151">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -3066,6 +3066,212 @@
         <charset val="129"/>
       </rPr>
       <t>구축</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>모임등록</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> UseCase </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>코드작업</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.11.15</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Everytime </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>연동</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>관련</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>코드</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작업</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.12.1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.12.3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>코드 수정</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.12.04</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">DB boundary </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>함수</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>구현</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">피드백 부분 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Test Scenario </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">작성, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">SRS </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -5422,8 +5628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
@@ -5971,13 +6177,25 @@
         <v>142</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="13"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="3"/>
+    <row r="30" spans="1:6" ht="15">
+      <c r="A30" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D30" s="8">
+        <v>0</v>
+      </c>
+      <c r="E30" s="16">
+        <v>220</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="13"/>
@@ -6534,8 +6752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
@@ -6740,52 +6958,124 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="13"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="3"/>
+      <c r="A13" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0</v>
+      </c>
+      <c r="E13" s="16">
+        <v>120</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="13"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="3"/>
+      <c r="A14" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0</v>
+      </c>
+      <c r="E14" s="16">
+        <v>140</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="13"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="3"/>
+      <c r="A15" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.95138888888888884</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0</v>
+      </c>
+      <c r="E15" s="16">
+        <v>170</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="13"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="3"/>
+      <c r="A16" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0</v>
+      </c>
+      <c r="E16" s="16">
+        <v>50</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="13"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="3"/>
+      <c r="A17" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0</v>
+      </c>
+      <c r="E17" s="16">
+        <v>120</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="13"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="18"/>
+      <c r="A18" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="D18" s="8">
+        <v>0</v>
+      </c>
+      <c r="E18" s="16">
+        <v>110</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="13"/>

</xml_diff>

<commit_message>
2019.12.07 김동욱 PSP 추가
</commit_message>
<xml_diff>
--- a/4팀_PSP_Sheet.xlsx
+++ b/4팀_PSP_Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\filling-good\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsung\Desktop\강의 등\github\filling good\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C5B83B-0705-4EE6-920D-FFE934D44797}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D44258-F37C-427B-97B1-C1F448A6423E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="총합" sheetId="1" r:id="rId1"/>
@@ -1480,7 +1480,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="164">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -3324,6 +3324,58 @@
   </si>
   <si>
     <t>11월 9일</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>장소 추천 안드로이드 스튜디오 코드 작성</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GUI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>구성</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 코드 파악 및 추천 코드 수정</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GUI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">구성에 따라 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>추천 코드 통합</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3549,7 +3601,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -3626,6 +3678,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="176" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="백분율" xfId="1" builtinId="5"/>
@@ -4016,16 +4069,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="46.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="46.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="11.85" customHeight="1">
+    <row r="1" spans="1:6" ht="11.9" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4037,7 +4090,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="11.85" customHeight="1">
+    <row r="2" spans="1:6" ht="11.9" customHeight="1">
       <c r="A2" s="20"/>
     </row>
     <row r="3" spans="1:6" ht="17.25" customHeight="1">
@@ -4052,8 +4105,8 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:6" ht="11.85" customHeight="1"/>
-    <row r="5" spans="1:6" s="10" customFormat="1" ht="26.4">
+    <row r="4" spans="1:6" ht="11.9" customHeight="1"/>
+    <row r="5" spans="1:6" s="10" customFormat="1" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -4354,7 +4407,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4371,7 +4424,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4388,7 +4441,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4405,7 +4458,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4422,7 +4475,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4439,7 +4492,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4456,7 +4509,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4472,18 +4525,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="49.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" customWidth="1"/>
+    <col min="6" max="6" width="49.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4500,7 +4553,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -4518,7 +4571,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -4538,7 +4591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6" ht="13">
       <c r="A6" s="13">
         <v>43733</v>
       </c>
@@ -4558,7 +4611,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.8">
+    <row r="7" spans="1:6" ht="13">
       <c r="A7" s="13">
         <v>43735</v>
       </c>
@@ -4578,7 +4631,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.8">
+    <row r="8" spans="1:6" ht="13">
       <c r="A8" s="13">
         <v>43742</v>
       </c>
@@ -4598,7 +4651,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.8">
+    <row r="9" spans="1:6" ht="13">
       <c r="A9" s="13">
         <v>43743</v>
       </c>
@@ -4618,7 +4671,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.8">
+    <row r="10" spans="1:6" ht="13">
       <c r="A10" s="13">
         <v>43744</v>
       </c>
@@ -4678,7 +4731,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.8">
+    <row r="13" spans="1:6" ht="13">
       <c r="A13" s="13">
         <v>43776</v>
       </c>
@@ -4698,7 +4751,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6">
+    <row r="14" spans="1:6" ht="16">
       <c r="A14" s="13">
         <v>43778</v>
       </c>
@@ -4718,7 +4771,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.6">
+    <row r="15" spans="1:6" ht="16">
       <c r="A15" s="13">
         <v>43781</v>
       </c>
@@ -4738,7 +4791,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6">
+    <row r="16" spans="1:6" ht="16">
       <c r="A16" s="13">
         <v>43782</v>
       </c>
@@ -4758,7 +4811,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.6">
+    <row r="17" spans="1:6" ht="16">
       <c r="A17" s="13">
         <v>43791</v>
       </c>
@@ -4778,7 +4831,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6" ht="13">
       <c r="A18" s="13">
         <v>43792</v>
       </c>
@@ -4798,7 +4851,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.8">
+    <row r="19" spans="1:6" ht="13">
       <c r="A19" s="13">
         <v>43793</v>
       </c>
@@ -4818,7 +4871,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.8">
+    <row r="20" spans="1:6" ht="13">
       <c r="A20" s="13">
         <v>43794</v>
       </c>
@@ -4838,7 +4891,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6" ht="13">
       <c r="A21" s="13">
         <v>43795</v>
       </c>
@@ -4858,53 +4911,125 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="13"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="13"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="13"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="13"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="13"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="13"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="3"/>
+    <row r="22" spans="1:6" ht="13">
+      <c r="A22" s="13">
+        <v>43796</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0</v>
+      </c>
+      <c r="E22" s="16">
+        <v>240</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="13">
+      <c r="A23" s="13">
+        <v>43797</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0</v>
+      </c>
+      <c r="E23" s="16">
+        <v>120</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="13">
+      <c r="A24" s="13">
+        <v>43800</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="8">
+        <v>0</v>
+      </c>
+      <c r="E24" s="16">
+        <v>240</v>
+      </c>
+      <c r="F24" s="44" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="13">
+      <c r="A25" s="13">
+        <v>43801</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D25" s="8">
+        <v>120</v>
+      </c>
+      <c r="E25" s="16">
+        <v>360</v>
+      </c>
+      <c r="F25" s="44" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16">
+      <c r="A26" s="13">
+        <v>43804</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D26" s="8">
+        <v>0</v>
+      </c>
+      <c r="E26" s="16">
+        <v>240</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16">
+      <c r="A27" s="13">
+        <v>43805</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="8">
+        <v>0</v>
+      </c>
+      <c r="E27" s="16">
+        <v>180</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="13"/>
@@ -5013,14 +5138,14 @@
       <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="42.44140625" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="42.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5037,7 +5162,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -5055,7 +5180,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -5075,7 +5200,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.6">
+    <row r="6" spans="1:6" ht="16">
       <c r="A6" s="13" t="s">
         <v>16</v>
       </c>
@@ -5095,7 +5220,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.6">
+    <row r="7" spans="1:6" ht="16">
       <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
@@ -5115,7 +5240,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.6">
+    <row r="8" spans="1:6" ht="16">
       <c r="A8" s="13" t="s">
         <v>15</v>
       </c>
@@ -5135,7 +5260,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.6">
+    <row r="9" spans="1:6" ht="16">
       <c r="A9" s="13" t="s">
         <v>60</v>
       </c>
@@ -5155,7 +5280,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.6">
+    <row r="10" spans="1:6" ht="16">
       <c r="A10" s="13" t="s">
         <v>62</v>
       </c>
@@ -5176,7 +5301,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6">
+    <row r="11" spans="1:6" ht="16">
       <c r="A11" s="13" t="s">
         <v>23</v>
       </c>
@@ -5216,7 +5341,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.6">
+    <row r="13" spans="1:6" ht="16">
       <c r="A13" s="14" t="s">
         <v>30</v>
       </c>
@@ -5236,7 +5361,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6">
+    <row r="14" spans="1:6" ht="16">
       <c r="A14" s="13" t="s">
         <v>53</v>
       </c>
@@ -5256,7 +5381,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.6">
+    <row r="15" spans="1:6" ht="16">
       <c r="A15" s="13" t="s">
         <v>48</v>
       </c>
@@ -5276,7 +5401,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6">
+    <row r="16" spans="1:6" ht="16">
       <c r="A16" s="13" t="s">
         <v>56</v>
       </c>
@@ -5336,7 +5461,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.6">
+    <row r="19" spans="1:6" ht="16">
       <c r="A19" s="13" t="s">
         <v>81</v>
       </c>
@@ -5356,7 +5481,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.6">
+    <row r="20" spans="1:6" ht="16">
       <c r="A20" s="13" t="s">
         <v>83</v>
       </c>
@@ -5376,7 +5501,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.6">
+    <row r="21" spans="1:6" ht="16">
       <c r="A21" s="13" t="s">
         <v>85</v>
       </c>
@@ -5396,7 +5521,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="28.8">
+    <row r="22" spans="1:6" ht="28.5">
       <c r="A22" s="13" t="s">
         <v>92</v>
       </c>
@@ -5416,7 +5541,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.6">
+    <row r="23" spans="1:6" ht="16">
       <c r="A23" s="13" t="s">
         <v>94</v>
       </c>
@@ -5436,7 +5561,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.6">
+    <row r="24" spans="1:6" ht="16">
       <c r="A24" s="13" t="s">
         <v>97</v>
       </c>
@@ -5456,7 +5581,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.6">
+    <row r="25" spans="1:6" ht="16">
       <c r="A25" s="13" t="s">
         <v>97</v>
       </c>
@@ -5476,7 +5601,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.6">
+    <row r="26" spans="1:6" ht="16">
       <c r="A26" s="13" t="s">
         <v>104</v>
       </c>
@@ -5496,7 +5621,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.6">
+    <row r="27" spans="1:6" ht="16">
       <c r="A27" s="13" t="s">
         <v>104</v>
       </c>
@@ -5516,7 +5641,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.6">
+    <row r="28" spans="1:6" ht="16">
       <c r="A28" s="13" t="s">
         <v>108</v>
       </c>
@@ -5536,7 +5661,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.6">
+    <row r="29" spans="1:6" ht="16">
       <c r="A29" s="13" t="s">
         <v>114</v>
       </c>
@@ -5556,7 +5681,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.6">
+    <row r="30" spans="1:6" ht="16">
       <c r="A30" s="13" t="s">
         <v>115</v>
       </c>
@@ -5636,7 +5761,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.6">
+    <row r="34" spans="1:6" ht="16">
       <c r="A34" s="13" t="s">
         <v>121</v>
       </c>
@@ -5656,7 +5781,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.6">
+    <row r="35" spans="1:6" ht="16">
       <c r="A35" s="13" t="s">
         <v>123</v>
       </c>
@@ -5676,7 +5801,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="31.2">
+    <row r="36" spans="1:6" ht="32">
       <c r="A36" s="13" t="s">
         <v>135</v>
       </c>
@@ -5696,7 +5821,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.6">
+    <row r="37" spans="1:6" ht="16">
       <c r="A37" s="3" t="s">
         <v>156</v>
       </c>
@@ -5716,7 +5841,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.6">
+    <row r="38" spans="1:6" ht="16">
       <c r="A38" s="38" t="s">
         <v>157</v>
       </c>
@@ -5775,14 +5900,14 @@
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="41.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="6" max="6" width="41.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5799,7 +5924,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -5817,7 +5942,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -5837,7 +5962,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6" ht="13">
       <c r="A6" s="13" t="s">
         <v>18</v>
       </c>
@@ -5857,7 +5982,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.8">
+    <row r="7" spans="1:6" ht="13">
       <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
@@ -5877,7 +6002,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.8">
+    <row r="8" spans="1:6" ht="13">
       <c r="A8" s="13" t="s">
         <v>21</v>
       </c>
@@ -5897,7 +6022,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.6">
+    <row r="9" spans="1:6" ht="16">
       <c r="A9" s="13" t="s">
         <v>62</v>
       </c>
@@ -5918,7 +6043,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.8">
+    <row r="10" spans="1:6" ht="13">
       <c r="A10" s="13" t="s">
         <v>23</v>
       </c>
@@ -5938,7 +6063,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6">
+    <row r="11" spans="1:6" ht="16">
       <c r="A11" s="13" t="s">
         <v>26</v>
       </c>
@@ -5958,7 +6083,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.8">
+    <row r="12" spans="1:6" ht="13">
       <c r="A12" s="14" t="s">
         <v>48</v>
       </c>
@@ -5978,7 +6103,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.8">
+    <row r="13" spans="1:6" ht="13">
       <c r="A13" s="13" t="s">
         <v>50</v>
       </c>
@@ -5999,7 +6124,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.8">
+    <row r="14" spans="1:6" ht="13">
       <c r="A14" s="13" t="s">
         <v>73</v>
       </c>
@@ -6019,7 +6144,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.8">
+    <row r="15" spans="1:6" ht="13">
       <c r="A15" s="13" t="s">
         <v>75</v>
       </c>
@@ -6039,7 +6164,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6">
+    <row r="16" spans="1:6" ht="16">
       <c r="A16" s="13" t="s">
         <v>85</v>
       </c>
@@ -6059,7 +6184,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.8">
+    <row r="17" spans="1:6" ht="13">
       <c r="A17" s="13" t="s">
         <v>87</v>
       </c>
@@ -6079,7 +6204,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6" ht="13">
       <c r="A18" s="13" t="s">
         <v>87</v>
       </c>
@@ -6099,7 +6224,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.8">
+    <row r="19" spans="1:6" ht="13">
       <c r="A19" s="13" t="s">
         <v>87</v>
       </c>
@@ -6119,7 +6244,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.8">
+    <row r="20" spans="1:6" ht="13">
       <c r="A20" s="13" t="s">
         <v>87</v>
       </c>
@@ -6139,7 +6264,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6" ht="13">
       <c r="A21" s="13" t="s">
         <v>100</v>
       </c>
@@ -6159,7 +6284,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.8">
+    <row r="22" spans="1:6" ht="13">
       <c r="A22" s="13" t="s">
         <v>100</v>
       </c>
@@ -6180,7 +6305,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="13.8">
+    <row r="23" spans="1:6" ht="13">
       <c r="A23" s="13" t="s">
         <v>110</v>
       </c>
@@ -6200,7 +6325,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="13.8">
+    <row r="24" spans="1:6" ht="13">
       <c r="A24" s="13" t="s">
         <v>112</v>
       </c>
@@ -6221,7 +6346,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="13.8">
+    <row r="25" spans="1:6" ht="13">
       <c r="A25" s="13" t="s">
         <v>128</v>
       </c>
@@ -6241,7 +6366,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="13.8">
+    <row r="26" spans="1:6" ht="13">
       <c r="A26" s="13" t="s">
         <v>130</v>
       </c>
@@ -6261,7 +6386,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="13.8">
+    <row r="27" spans="1:6" ht="13">
       <c r="A27" s="13" t="s">
         <v>130</v>
       </c>
@@ -6281,7 +6406,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="13.8">
+    <row r="28" spans="1:6" ht="13">
       <c r="A28" s="13" t="s">
         <v>133</v>
       </c>
@@ -6301,7 +6426,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="13.8">
+    <row r="29" spans="1:6" ht="13">
       <c r="A29" s="13" t="s">
         <v>137</v>
       </c>
@@ -6321,7 +6446,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="13.8">
+    <row r="30" spans="1:6" ht="13">
       <c r="A30" s="13" t="s">
         <v>138</v>
       </c>
@@ -6341,7 +6466,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="13.8">
+    <row r="31" spans="1:6" ht="13">
       <c r="A31" s="13" t="s">
         <v>141</v>
       </c>
@@ -6361,7 +6486,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.6">
+    <row r="32" spans="1:6" ht="16">
       <c r="A32" s="13" t="s">
         <v>149</v>
       </c>
@@ -6381,7 +6506,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="13.8">
+    <row r="33" spans="1:6" ht="13">
       <c r="A33" s="3" t="s">
         <v>151</v>
       </c>
@@ -6401,7 +6526,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="13.8">
+    <row r="34" spans="1:6" ht="13">
       <c r="A34" s="13" t="s">
         <v>154</v>
       </c>
@@ -6489,13 +6614,13 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="4" max="4" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="52.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" customWidth="1"/>
+    <col min="6" max="6" width="52.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -6512,7 +6637,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="13.8">
+    <row r="3" spans="1:7" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -6530,7 +6655,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="26.4">
+    <row r="5" spans="1:7" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -6550,7 +6675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="13.8">
+    <row r="6" spans="1:7" ht="13">
       <c r="A6" s="13">
         <v>43733</v>
       </c>
@@ -6698,7 +6823,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.6">
+    <row r="13" spans="1:7" ht="16">
       <c r="A13" s="13">
         <v>43741</v>
       </c>
@@ -6761,7 +6886,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.6">
+    <row r="16" spans="1:7" ht="16">
       <c r="A16" s="43" t="s">
         <v>160</v>
       </c>
@@ -6789,7 +6914,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6" ht="13">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -6813,7 +6938,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6" ht="13">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -6972,17 +7097,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="50.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -6999,7 +7124,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -7017,7 +7142,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -7037,7 +7162,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6" ht="13">
       <c r="A6" s="13" t="s">
         <v>63</v>
       </c>
@@ -7057,7 +7182,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.8">
+    <row r="7" spans="1:6" ht="13">
       <c r="A7" s="13" t="s">
         <v>65</v>
       </c>
@@ -7077,7 +7202,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.8">
+    <row r="8" spans="1:6" ht="13">
       <c r="A8" s="13" t="s">
         <v>67</v>
       </c>
@@ -7097,7 +7222,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.6">
+    <row r="9" spans="1:6" ht="16">
       <c r="A9" s="13" t="s">
         <v>62</v>
       </c>
@@ -7118,7 +7243,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.8">
+    <row r="10" spans="1:6" ht="13">
       <c r="A10" s="13" t="s">
         <v>69</v>
       </c>
@@ -7138,7 +7263,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.8">
+    <row r="11" spans="1:6" ht="13">
       <c r="A11" s="13" t="s">
         <v>71</v>
       </c>
@@ -7158,7 +7283,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.6">
+    <row r="12" spans="1:6" ht="16">
       <c r="A12" s="14" t="s">
         <v>30</v>
       </c>
@@ -7198,7 +7323,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6">
+    <row r="14" spans="1:6" ht="16">
       <c r="A14" s="13" t="s">
         <v>85</v>
       </c>
@@ -7218,7 +7343,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.8">
+    <row r="15" spans="1:6" ht="13">
       <c r="A15" s="13" t="s">
         <v>97</v>
       </c>
@@ -7238,7 +7363,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13.8">
+    <row r="16" spans="1:6" ht="13">
       <c r="A16" s="13" t="s">
         <v>144</v>
       </c>
@@ -7258,7 +7383,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.8">
+    <row r="17" spans="1:6" ht="13">
       <c r="A17" s="13" t="s">
         <v>118</v>
       </c>
@@ -7278,7 +7403,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6" ht="13">
       <c r="A18" s="13" t="s">
         <v>120</v>
       </c>
@@ -7298,7 +7423,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.8">
+    <row r="19" spans="1:6" ht="13">
       <c r="A19" s="13" t="s">
         <v>146</v>
       </c>
@@ -7318,7 +7443,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.8">
+    <row r="20" spans="1:6" ht="13">
       <c r="A20" s="13" t="s">
         <v>147</v>
       </c>
@@ -7354,7 +7479,7 @@
       <c r="E22" s="16"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" ht="13.8">
+    <row r="23" spans="1:6" ht="13">
       <c r="A23" s="13"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -7517,7 +7642,7 @@
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7534,7 +7659,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7551,7 +7676,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
2019.12.10 김동욱 PSP update
</commit_message>
<xml_diff>
--- a/4팀_PSP_Sheet.xlsx
+++ b/4팀_PSP_Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\filling-good\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsung\Desktop\강의 등\github\filling good\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506F2725-CC9F-4FFC-9833-9A0C03ED90D9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147463AB-E79F-4812-B32F-150DA411E462}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3444" yWindow="3384" windowWidth="17208" windowHeight="8976" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="총합" sheetId="1" r:id="rId1"/>
@@ -1483,7 +1483,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="223">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -4343,6 +4343,21 @@
   </si>
   <si>
     <t>GUI, SRS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>추천</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 부분 test case 작성 및 서류 정리 작업</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -5183,16 +5198,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="46.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="46.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="11.85" customHeight="1">
+    <row r="1" spans="1:6" ht="11.9" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5204,7 +5219,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="11.85" customHeight="1">
+    <row r="2" spans="1:6" ht="11.9" customHeight="1">
       <c r="A2" s="20"/>
     </row>
     <row r="3" spans="1:6" ht="17.25" customHeight="1">
@@ -5219,8 +5234,8 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:6" ht="11.85" customHeight="1"/>
-    <row r="5" spans="1:6" s="10" customFormat="1" ht="26.4">
+    <row r="4" spans="1:6" ht="11.9" customHeight="1"/>
+    <row r="5" spans="1:6" s="10" customFormat="1" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -5521,7 +5536,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5538,7 +5553,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5555,7 +5570,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5572,7 +5587,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5589,7 +5604,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5606,7 +5621,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5623,7 +5638,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5639,18 +5654,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="49.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" customWidth="1"/>
+    <col min="6" max="6" width="49.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5667,7 +5682,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -5685,7 +5700,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -5705,7 +5720,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6" ht="13">
       <c r="A6" s="13">
         <v>43733</v>
       </c>
@@ -5725,7 +5740,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.8">
+    <row r="7" spans="1:6" ht="13">
       <c r="A7" s="13">
         <v>43735</v>
       </c>
@@ -5745,7 +5760,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.8">
+    <row r="8" spans="1:6" ht="13">
       <c r="A8" s="13">
         <v>43742</v>
       </c>
@@ -5765,7 +5780,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.8">
+    <row r="9" spans="1:6" ht="13">
       <c r="A9" s="13">
         <v>43743</v>
       </c>
@@ -5785,7 +5800,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.8">
+    <row r="10" spans="1:6" ht="13">
       <c r="A10" s="13">
         <v>43744</v>
       </c>
@@ -5845,7 +5860,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.8">
+    <row r="13" spans="1:6" ht="13">
       <c r="A13" s="13">
         <v>43776</v>
       </c>
@@ -5865,7 +5880,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6">
+    <row r="14" spans="1:6" ht="16">
       <c r="A14" s="13">
         <v>43778</v>
       </c>
@@ -5885,7 +5900,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.6">
+    <row r="15" spans="1:6" ht="16">
       <c r="A15" s="13">
         <v>43781</v>
       </c>
@@ -5905,7 +5920,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6">
+    <row r="16" spans="1:6" ht="16">
       <c r="A16" s="13">
         <v>43782</v>
       </c>
@@ -5925,7 +5940,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.6">
+    <row r="17" spans="1:6" ht="16">
       <c r="A17" s="13">
         <v>43791</v>
       </c>
@@ -5945,7 +5960,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6" ht="13">
       <c r="A18" s="13">
         <v>43792</v>
       </c>
@@ -5965,7 +5980,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.8">
+    <row r="19" spans="1:6" ht="13">
       <c r="A19" s="13">
         <v>43793</v>
       </c>
@@ -5985,7 +6000,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.8">
+    <row r="20" spans="1:6" ht="13">
       <c r="A20" s="13">
         <v>43794</v>
       </c>
@@ -6005,7 +6020,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6" ht="13">
       <c r="A21" s="13">
         <v>43795</v>
       </c>
@@ -6025,7 +6040,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.8">
+    <row r="22" spans="1:6" ht="13">
       <c r="A22" s="13">
         <v>43796</v>
       </c>
@@ -6045,7 +6060,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="13.8">
+    <row r="23" spans="1:6" ht="13">
       <c r="A23" s="13">
         <v>43797</v>
       </c>
@@ -6065,7 +6080,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="13.8">
+    <row r="24" spans="1:6" ht="13">
       <c r="A24" s="13">
         <v>43800</v>
       </c>
@@ -6085,7 +6100,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="13.8">
+    <row r="25" spans="1:6" ht="13">
       <c r="A25" s="13">
         <v>43801</v>
       </c>
@@ -6105,7 +6120,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.6">
+    <row r="26" spans="1:6" ht="16">
       <c r="A26" s="13">
         <v>43804</v>
       </c>
@@ -6125,7 +6140,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.6">
+    <row r="27" spans="1:6" ht="16">
       <c r="A27" s="13">
         <v>43805</v>
       </c>
@@ -6145,7 +6160,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.6">
+    <row r="28" spans="1:6" ht="16">
       <c r="A28" s="13">
         <v>43806</v>
       </c>
@@ -6165,7 +6180,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.6">
+    <row r="29" spans="1:6" ht="16">
       <c r="A29" s="13">
         <v>43807</v>
       </c>
@@ -6185,7 +6200,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.6">
+    <row r="30" spans="1:6" ht="16">
       <c r="A30" s="13">
         <v>43807</v>
       </c>
@@ -6205,7 +6220,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.6">
+    <row r="31" spans="1:6" ht="16">
       <c r="A31" s="13">
         <v>43807</v>
       </c>
@@ -6225,7 +6240,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.6">
+    <row r="32" spans="1:6" ht="16">
       <c r="A32" s="13">
         <v>43808</v>
       </c>
@@ -6245,7 +6260,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.6">
+    <row r="33" spans="1:6" ht="16">
       <c r="A33" s="13">
         <v>43808</v>
       </c>
@@ -6265,21 +6280,45 @@
         <v>219</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="13"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="13"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="3"/>
+    <row r="34" spans="1:6" ht="16">
+      <c r="A34" s="13">
+        <v>43808</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1</v>
+      </c>
+      <c r="D34" s="8">
+        <v>60</v>
+      </c>
+      <c r="E34" s="16">
+        <v>300</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="13">
+      <c r="A35" s="13">
+        <v>43809</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="D35" s="8">
+        <v>0</v>
+      </c>
+      <c r="E35" s="16">
+        <v>180</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="13"/>
@@ -6320,18 +6359,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="42.44140625" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="42.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -6348,7 +6387,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -6366,7 +6405,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -6386,7 +6425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.6">
+    <row r="6" spans="1:6" ht="16">
       <c r="A6" s="13" t="s">
         <v>16</v>
       </c>
@@ -6406,7 +6445,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.6">
+    <row r="7" spans="1:6" ht="16">
       <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
@@ -6426,7 +6465,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.6">
+    <row r="8" spans="1:6" ht="16">
       <c r="A8" s="13" t="s">
         <v>15</v>
       </c>
@@ -6446,7 +6485,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.6">
+    <row r="9" spans="1:6" ht="16">
       <c r="A9" s="13" t="s">
         <v>60</v>
       </c>
@@ -6466,7 +6505,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.6">
+    <row r="10" spans="1:6" ht="16">
       <c r="A10" s="13" t="s">
         <v>62</v>
       </c>
@@ -6487,7 +6526,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6">
+    <row r="11" spans="1:6" ht="16">
       <c r="A11" s="13" t="s">
         <v>23</v>
       </c>
@@ -6527,7 +6566,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.6">
+    <row r="13" spans="1:6" ht="16">
       <c r="A13" s="14" t="s">
         <v>30</v>
       </c>
@@ -6547,7 +6586,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6">
+    <row r="14" spans="1:6" ht="16">
       <c r="A14" s="13" t="s">
         <v>53</v>
       </c>
@@ -6567,7 +6606,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.6">
+    <row r="15" spans="1:6" ht="16">
       <c r="A15" s="13" t="s">
         <v>48</v>
       </c>
@@ -6587,7 +6626,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6">
+    <row r="16" spans="1:6" ht="16">
       <c r="A16" s="13" t="s">
         <v>56</v>
       </c>
@@ -6647,7 +6686,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.6">
+    <row r="19" spans="1:6" ht="16">
       <c r="A19" s="13" t="s">
         <v>81</v>
       </c>
@@ -6667,7 +6706,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.6">
+    <row r="20" spans="1:6" ht="16">
       <c r="A20" s="13" t="s">
         <v>83</v>
       </c>
@@ -6687,7 +6726,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.6">
+    <row r="21" spans="1:6" ht="16">
       <c r="A21" s="13" t="s">
         <v>85</v>
       </c>
@@ -6707,7 +6746,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="28.8">
+    <row r="22" spans="1:6" ht="28.5">
       <c r="A22" s="13" t="s">
         <v>92</v>
       </c>
@@ -6727,7 +6766,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.6">
+    <row r="23" spans="1:6" ht="16">
       <c r="A23" s="13" t="s">
         <v>94</v>
       </c>
@@ -6747,7 +6786,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.6">
+    <row r="24" spans="1:6" ht="16">
       <c r="A24" s="13" t="s">
         <v>97</v>
       </c>
@@ -6767,7 +6806,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.6">
+    <row r="25" spans="1:6" ht="16">
       <c r="A25" s="13" t="s">
         <v>97</v>
       </c>
@@ -6787,7 +6826,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.6">
+    <row r="26" spans="1:6" ht="16">
       <c r="A26" s="13" t="s">
         <v>104</v>
       </c>
@@ -6807,7 +6846,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.6">
+    <row r="27" spans="1:6" ht="16">
       <c r="A27" s="13" t="s">
         <v>104</v>
       </c>
@@ -6827,7 +6866,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.6">
+    <row r="28" spans="1:6" ht="16">
       <c r="A28" s="13" t="s">
         <v>108</v>
       </c>
@@ -6847,7 +6886,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.6">
+    <row r="29" spans="1:6" ht="16">
       <c r="A29" s="13" t="s">
         <v>114</v>
       </c>
@@ -6867,7 +6906,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.6">
+    <row r="30" spans="1:6" ht="16">
       <c r="A30" s="13" t="s">
         <v>115</v>
       </c>
@@ -6947,7 +6986,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.6">
+    <row r="34" spans="1:6" ht="16">
       <c r="A34" s="13" t="s">
         <v>121</v>
       </c>
@@ -6967,7 +7006,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.6">
+    <row r="35" spans="1:6" ht="16">
       <c r="A35" s="13" t="s">
         <v>123</v>
       </c>
@@ -6987,7 +7026,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="31.2">
+    <row r="36" spans="1:6" ht="32">
       <c r="A36" s="13" t="s">
         <v>135</v>
       </c>
@@ -7007,7 +7046,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.6">
+    <row r="37" spans="1:6" ht="16">
       <c r="A37" s="3" t="s">
         <v>156</v>
       </c>
@@ -7027,7 +7066,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.6">
+    <row r="38" spans="1:6" ht="16">
       <c r="A38" s="38" t="s">
         <v>157</v>
       </c>
@@ -7067,7 +7106,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="31.2">
+    <row r="40" spans="1:6" ht="32">
       <c r="A40" s="46" t="s">
         <v>163</v>
       </c>
@@ -7087,7 +7126,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.6">
+    <row r="41" spans="1:6" ht="16">
       <c r="A41" s="48" t="s">
         <v>173</v>
       </c>
@@ -7107,7 +7146,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.6">
+    <row r="42" spans="1:6" ht="16">
       <c r="A42" s="49" t="s">
         <v>175</v>
       </c>
@@ -7127,7 +7166,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="31.2">
+    <row r="43" spans="1:6" ht="32">
       <c r="A43" s="60" t="s">
         <v>212</v>
       </c>
@@ -7206,14 +7245,14 @@
       <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="41.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="6" max="6" width="41.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -7230,7 +7269,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -7248,7 +7287,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -7268,7 +7307,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6" ht="13">
       <c r="A6" s="13" t="s">
         <v>18</v>
       </c>
@@ -7288,7 +7327,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.8">
+    <row r="7" spans="1:6" ht="13">
       <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
@@ -7308,7 +7347,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.8">
+    <row r="8" spans="1:6" ht="13">
       <c r="A8" s="13" t="s">
         <v>21</v>
       </c>
@@ -7328,7 +7367,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.6">
+    <row r="9" spans="1:6" ht="16">
       <c r="A9" s="13" t="s">
         <v>62</v>
       </c>
@@ -7349,7 +7388,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.8">
+    <row r="10" spans="1:6" ht="13">
       <c r="A10" s="13" t="s">
         <v>23</v>
       </c>
@@ -7369,7 +7408,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6">
+    <row r="11" spans="1:6" ht="16">
       <c r="A11" s="13" t="s">
         <v>26</v>
       </c>
@@ -7389,7 +7428,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.8">
+    <row r="12" spans="1:6" ht="13">
       <c r="A12" s="14" t="s">
         <v>48</v>
       </c>
@@ -7409,7 +7448,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.8">
+    <row r="13" spans="1:6" ht="13">
       <c r="A13" s="13" t="s">
         <v>50</v>
       </c>
@@ -7430,7 +7469,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.8">
+    <row r="14" spans="1:6" ht="13">
       <c r="A14" s="13" t="s">
         <v>73</v>
       </c>
@@ -7450,7 +7489,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.8">
+    <row r="15" spans="1:6" ht="13">
       <c r="A15" s="13" t="s">
         <v>75</v>
       </c>
@@ -7470,7 +7509,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6">
+    <row r="16" spans="1:6" ht="16">
       <c r="A16" s="13" t="s">
         <v>85</v>
       </c>
@@ -7490,7 +7529,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.8">
+    <row r="17" spans="1:6" ht="13">
       <c r="A17" s="13" t="s">
         <v>87</v>
       </c>
@@ -7510,7 +7549,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6" ht="13">
       <c r="A18" s="13" t="s">
         <v>87</v>
       </c>
@@ -7530,7 +7569,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.8">
+    <row r="19" spans="1:6" ht="13">
       <c r="A19" s="13" t="s">
         <v>87</v>
       </c>
@@ -7550,7 +7589,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.8">
+    <row r="20" spans="1:6" ht="13">
       <c r="A20" s="13" t="s">
         <v>87</v>
       </c>
@@ -7570,7 +7609,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6" ht="13">
       <c r="A21" s="13" t="s">
         <v>100</v>
       </c>
@@ -7590,7 +7629,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.8">
+    <row r="22" spans="1:6" ht="13">
       <c r="A22" s="13" t="s">
         <v>100</v>
       </c>
@@ -7611,7 +7650,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="13.8">
+    <row r="23" spans="1:6" ht="13">
       <c r="A23" s="13" t="s">
         <v>110</v>
       </c>
@@ -7631,7 +7670,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="13.8">
+    <row r="24" spans="1:6" ht="13">
       <c r="A24" s="13" t="s">
         <v>112</v>
       </c>
@@ -7652,7 +7691,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="13.8">
+    <row r="25" spans="1:6" ht="13">
       <c r="A25" s="13" t="s">
         <v>128</v>
       </c>
@@ -7672,7 +7711,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="13.8">
+    <row r="26" spans="1:6" ht="13">
       <c r="A26" s="13" t="s">
         <v>130</v>
       </c>
@@ -7692,7 +7731,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="13.8">
+    <row r="27" spans="1:6" ht="13">
       <c r="A27" s="13" t="s">
         <v>130</v>
       </c>
@@ -7712,7 +7751,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="13.8">
+    <row r="28" spans="1:6" ht="13">
       <c r="A28" s="13" t="s">
         <v>133</v>
       </c>
@@ -7732,7 +7771,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="13.8">
+    <row r="29" spans="1:6" ht="13">
       <c r="A29" s="13" t="s">
         <v>137</v>
       </c>
@@ -7752,7 +7791,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="13.8">
+    <row r="30" spans="1:6" ht="13">
       <c r="A30" s="13" t="s">
         <v>138</v>
       </c>
@@ -7772,7 +7811,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="13.8">
+    <row r="31" spans="1:6" ht="13">
       <c r="A31" s="13" t="s">
         <v>141</v>
       </c>
@@ -7792,7 +7831,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.6">
+    <row r="32" spans="1:6" ht="16">
       <c r="A32" s="13" t="s">
         <v>149</v>
       </c>
@@ -7812,7 +7851,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="13.8">
+    <row r="33" spans="1:6" ht="13">
       <c r="A33" s="3" t="s">
         <v>151</v>
       </c>
@@ -7832,7 +7871,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="13.8">
+    <row r="34" spans="1:6" ht="13">
       <c r="A34" s="13" t="s">
         <v>154</v>
       </c>
@@ -7852,7 +7891,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="13.8">
+    <row r="35" spans="1:6" ht="13">
       <c r="A35" s="13" t="s">
         <v>165</v>
       </c>
@@ -7872,7 +7911,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="13.8">
+    <row r="36" spans="1:6" ht="13">
       <c r="A36" s="13" t="s">
         <v>171</v>
       </c>
@@ -7892,7 +7931,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.6">
+    <row r="37" spans="1:6" ht="16">
       <c r="A37" s="13" t="s">
         <v>210</v>
       </c>
@@ -7912,7 +7951,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="13.8">
+    <row r="38" spans="1:6" ht="13">
       <c r="A38" s="13" t="s">
         <v>214</v>
       </c>
@@ -7932,7 +7971,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="13.8">
+    <row r="39" spans="1:6" ht="13">
       <c r="A39" s="3" t="s">
         <v>216</v>
       </c>
@@ -7980,13 +8019,13 @@
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="4" max="4" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="52.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" customWidth="1"/>
+    <col min="6" max="6" width="52.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -8003,7 +8042,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="13.8">
+    <row r="3" spans="1:7" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -8021,7 +8060,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="26.4">
+    <row r="5" spans="1:7" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -8041,7 +8080,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="13.8">
+    <row r="6" spans="1:7" ht="13">
       <c r="A6" s="13">
         <v>43733</v>
       </c>
@@ -8189,7 +8228,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.6">
+    <row r="13" spans="1:7" ht="16">
       <c r="A13" s="13">
         <v>43741</v>
       </c>
@@ -8252,7 +8291,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.6">
+    <row r="16" spans="1:7" ht="16">
       <c r="A16" s="43" t="s">
         <v>198</v>
       </c>
@@ -8273,7 +8312,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.6">
+    <row r="17" spans="1:6" ht="16">
       <c r="A17" s="13" t="s">
         <v>199</v>
       </c>
@@ -8294,7 +8333,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6" ht="13">
       <c r="A18" s="13" t="s">
         <v>200</v>
       </c>
@@ -8315,7 +8354,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.6">
+    <row r="19" spans="1:6" ht="16">
       <c r="A19" s="43" t="s">
         <v>202</v>
       </c>
@@ -8336,7 +8375,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.8">
+    <row r="20" spans="1:6" ht="13">
       <c r="A20" s="13" t="s">
         <v>203</v>
       </c>
@@ -8357,7 +8396,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6" ht="13">
       <c r="A21" s="13" t="s">
         <v>201</v>
       </c>
@@ -8378,7 +8417,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.6">
+    <row r="22" spans="1:6" ht="16">
       <c r="A22" s="43" t="s">
         <v>204</v>
       </c>
@@ -8399,7 +8438,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.6">
+    <row r="23" spans="1:6" ht="16">
       <c r="A23" s="43" t="s">
         <v>205</v>
       </c>
@@ -8420,7 +8459,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.6">
+    <row r="24" spans="1:6" ht="16">
       <c r="A24" s="43" t="s">
         <v>205</v>
       </c>
@@ -8441,7 +8480,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.6">
+    <row r="25" spans="1:6" ht="16">
       <c r="A25" s="43">
         <v>43770</v>
       </c>
@@ -8462,7 +8501,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.6">
+    <row r="26" spans="1:6" ht="16">
       <c r="A26" s="13">
         <v>43771</v>
       </c>
@@ -8483,7 +8522,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.6">
+    <row r="27" spans="1:6" ht="16">
       <c r="A27" s="13">
         <v>43771</v>
       </c>
@@ -8504,7 +8543,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.6">
+    <row r="28" spans="1:6" ht="16">
       <c r="A28" s="43">
         <v>43772</v>
       </c>
@@ -8546,7 +8585,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.6">
+    <row r="30" spans="1:6" ht="16">
       <c r="A30" s="43">
         <v>43778</v>
       </c>
@@ -8567,7 +8606,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="13.8">
+    <row r="31" spans="1:6" ht="13">
       <c r="A31" s="13" t="s">
         <v>206</v>
       </c>
@@ -8588,7 +8627,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="13.8">
+    <row r="32" spans="1:6" ht="13">
       <c r="A32" s="13" t="s">
         <v>206</v>
       </c>
@@ -8609,7 +8648,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.6">
+    <row r="33" spans="1:6" ht="16">
       <c r="A33" s="13" t="s">
         <v>207</v>
       </c>
@@ -8630,7 +8669,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="13.8">
+    <row r="34" spans="1:6" ht="13">
       <c r="A34" s="13" t="s">
         <v>208</v>
       </c>
@@ -8651,7 +8690,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="13.8">
+    <row r="35" spans="1:6" ht="13">
       <c r="A35" s="13" t="s">
         <v>209</v>
       </c>
@@ -8672,7 +8711,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.6">
+    <row r="36" spans="1:6" ht="16">
       <c r="A36" s="13">
         <v>43800</v>
       </c>
@@ -8735,7 +8774,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.6">
+    <row r="39" spans="1:6" ht="16">
       <c r="A39" s="13">
         <v>43806</v>
       </c>
@@ -8796,13 +8835,13 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="50.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -8819,7 +8858,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -8837,7 +8876,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="26">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -8857,7 +8896,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6" ht="13">
       <c r="A6" s="13" t="s">
         <v>63</v>
       </c>
@@ -8877,7 +8916,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.8">
+    <row r="7" spans="1:6" ht="13">
       <c r="A7" s="13" t="s">
         <v>65</v>
       </c>
@@ -8897,7 +8936,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.8">
+    <row r="8" spans="1:6" ht="13">
       <c r="A8" s="13" t="s">
         <v>67</v>
       </c>
@@ -8917,7 +8956,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.6">
+    <row r="9" spans="1:6" ht="16">
       <c r="A9" s="13" t="s">
         <v>62</v>
       </c>
@@ -8938,7 +8977,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.8">
+    <row r="10" spans="1:6" ht="13">
       <c r="A10" s="13" t="s">
         <v>69</v>
       </c>
@@ -8958,7 +8997,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.8">
+    <row r="11" spans="1:6" ht="13">
       <c r="A11" s="13" t="s">
         <v>71</v>
       </c>
@@ -8978,7 +9017,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.6">
+    <row r="12" spans="1:6" ht="16">
       <c r="A12" s="14" t="s">
         <v>30</v>
       </c>
@@ -9018,7 +9057,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6">
+    <row r="14" spans="1:6" ht="16">
       <c r="A14" s="13" t="s">
         <v>85</v>
       </c>
@@ -9038,7 +9077,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.8">
+    <row r="15" spans="1:6" ht="13">
       <c r="A15" s="13" t="s">
         <v>97</v>
       </c>
@@ -9058,7 +9097,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13.8">
+    <row r="16" spans="1:6" ht="13">
       <c r="A16" s="13" t="s">
         <v>144</v>
       </c>
@@ -9078,7 +9117,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.8">
+    <row r="17" spans="1:6" ht="13">
       <c r="A17" s="13" t="s">
         <v>118</v>
       </c>
@@ -9098,7 +9137,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6" ht="13">
       <c r="A18" s="13" t="s">
         <v>120</v>
       </c>
@@ -9118,7 +9157,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.8">
+    <row r="19" spans="1:6" ht="13">
       <c r="A19" s="13" t="s">
         <v>146</v>
       </c>
@@ -9138,7 +9177,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.8">
+    <row r="20" spans="1:6" ht="13">
       <c r="A20" s="13" t="s">
         <v>147</v>
       </c>
@@ -9158,7 +9197,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6" ht="13">
       <c r="A21" s="13" t="s">
         <v>167</v>
       </c>
@@ -9178,7 +9217,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.8">
+    <row r="22" spans="1:6" ht="13">
       <c r="A22" s="13" t="s">
         <v>169</v>
       </c>
@@ -9198,7 +9237,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="13.8">
+    <row r="23" spans="1:6" ht="13">
       <c r="A23" s="13"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -9361,7 +9400,7 @@
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9378,7 +9417,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9395,7 +9434,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>